<commit_message>
Updated TAM template and TAM exporter
</commit_message>
<xml_diff>
--- a/xls/templates/tam-template.xlsx
+++ b/xls/templates/tam-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA0B83B-0463-AD4D-A383-5A541C938C9C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BC3FC3-8856-E447-9627-3CAB3A8AB5F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="33260" windowHeight="20440" activeTab="2" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
+    <workbookView xWindow="-380" yWindow="460" windowWidth="33260" windowHeight="20440" activeTab="2" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Zip Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
   <si>
     <t>Rent Stats</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>2024</t>
+  </si>
+  <si>
+    <t>Total Population</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -469,8 +472,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +497,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -497,15 +512,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -532,14 +548,17 @@
     <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="5"/>
-    <xf numFmtId="6" fontId="10" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -875,10 +894,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -908,11 +927,11 @@
       <c r="C4" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1213,10 +1232,10 @@
       <c r="D32" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1621,30 +1640,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059DB5A-4215-0640-95EF-B3BB098332D1}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4">
@@ -1679,7 +1698,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="26">
         <f>ROUND('Sample Zip Data'!B8*(1+'Static Data'!B10),0)</f>
         <v>1827</v>
       </c>
@@ -1720,7 +1739,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="26">
         <f>ROUND('Sample Zip Data'!B9*(1+'Static Data'!B11),0)</f>
         <v>3893</v>
       </c>
@@ -1761,7 +1780,7 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="26">
         <f>ROUND('Sample Zip Data'!B10*(1+'Static Data'!B12),0)</f>
         <v>3276</v>
       </c>
@@ -1802,7 +1821,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="26">
         <f>ROUND('Sample Zip Data'!B11*(1+'Static Data'!B13),0)</f>
         <v>3449</v>
       </c>
@@ -1843,7 +1862,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="26">
         <f>ROUND('Sample Zip Data'!B12*(1+'Static Data'!B14),0)</f>
         <v>2512</v>
       </c>
@@ -1884,7 +1903,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="26">
         <f>ROUND('Sample Zip Data'!B13*(1+'Static Data'!B15),0)</f>
         <v>2587</v>
       </c>
@@ -1922,17 +1941,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -1968,7 +1987,7 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="26">
         <f>ROUND(B3*SUM($B$29:$B$31),0)</f>
         <v>1315</v>
       </c>
@@ -2009,7 +2028,7 @@
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="26">
         <f t="shared" ref="B13:J17" si="1">ROUND(B4*SUM($B$29:$B$31),0)</f>
         <v>2803</v>
       </c>
@@ -2050,7 +2069,7 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="26">
         <f t="shared" si="1"/>
         <v>2359</v>
       </c>
@@ -2091,7 +2110,7 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="26">
         <f t="shared" si="1"/>
         <v>2483</v>
       </c>
@@ -2132,7 +2151,7 @@
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="26">
         <f t="shared" si="1"/>
         <v>1809</v>
       </c>
@@ -2173,7 +2192,7 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="26">
         <f t="shared" si="1"/>
         <v>1863</v>
       </c>
@@ -2211,13 +2230,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20">
@@ -2360,17 +2379,17 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="22"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="17"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25000</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="27">
         <v>0.12</v>
       </c>
       <c r="C29" s="2"/>
@@ -2379,7 +2398,7 @@
       <c r="A30">
         <v>35000</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="27">
         <v>0.15</v>
       </c>
       <c r="C30" s="2"/>
@@ -2388,24 +2407,23 @@
       <c r="A31" s="8">
         <v>45000</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="27">
         <v>0.45</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="17"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="5">
-        <f>SUM('Sample Zip Data'!B35:B37)</f>
-        <v>0.26866266999999999</v>
+        <v>0.6</v>
       </c>
       <c r="C34" s="16"/>
     </row>
@@ -2414,8 +2432,8 @@
         <v>57</v>
       </c>
       <c r="B35" s="5">
-        <f>SUM('Sample Zip Data'!B38:B39)</f>
-        <v>0.73133732000000007</v>
+        <f>1-B34</f>
+        <v>0.4</v>
       </c>
       <c r="C35" s="16"/>
     </row>
@@ -2425,18 +2443,19 @@
       </c>
       <c r="B36" s="5">
         <f>SUM(B34:B35)</f>
-        <v>0.99999999000000006</v>
+        <v>1</v>
       </c>
       <c r="C36" s="5"/>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="26">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2445,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36708BF2-1F90-C543-A265-0490C92231C9}">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2502,17 +2521,17 @@
         <v>66</v>
       </c>
       <c r="B6" s="3">
-        <f>'Sample Zip Data'!B7</f>
-        <v>21371</v>
+        <f>Computation!B38</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="3" t="e">
+      <c r="B7" s="3">
         <f>SUM(B95:B100)</f>
-        <v>#REF!</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -2528,9 +2547,9 @@
       <c r="A9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="3" t="e">
+      <c r="B9" s="3">
         <f>SUM(E95:E100)</f>
-        <v>#REF!</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -2546,7 +2565,7 @@
       <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="25">
         <v>950</v>
       </c>
       <c r="C12" s="20"/>
@@ -2555,7 +2574,7 @@
       <c r="A13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="25">
         <v>750</v>
       </c>
       <c r="C13" s="20"/>
@@ -2564,7 +2583,7 @@
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="25">
         <f>'Sample Zip Data'!B4</f>
         <v>778</v>
       </c>
@@ -2606,10 +2625,10 @@
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="22">
         <v>0</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="22">
         <v>0.12</v>
       </c>
       <c r="M18" s="4"/>
@@ -2622,10 +2641,10 @@
       <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="22">
         <v>0.12</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="22">
         <v>0.24</v>
       </c>
       <c r="M19" s="4"/>
@@ -2638,10 +2657,10 @@
       <c r="A20" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="22">
         <v>0.24</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>0.35</v>
       </c>
       <c r="M20" s="4"/>
@@ -2654,10 +2673,10 @@
       <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="22">
         <v>0.35</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="22">
         <v>0.45</v>
       </c>
       <c r="M21" s="4"/>
@@ -2670,10 +2689,10 @@
       <c r="A22" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="22">
         <v>0.45</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="22">
         <v>0.55000000000000004</v>
       </c>
       <c r="M22" s="4"/>
@@ -3301,15 +3320,15 @@
       </c>
       <c r="B38">
         <f>ROUND(B36*Computation!$B$34,0)</f>
-        <v>93</v>
+        <v>209</v>
       </c>
       <c r="C38">
-        <f>ROUND(C36*Computation!$C$34,0)</f>
-        <v>0</v>
+        <f>ROUND(C36*Computation!$B$34,0)</f>
+        <v>174</v>
       </c>
       <c r="D38">
-        <f>ROUND(D36*Computation!$C$34,0)</f>
-        <v>0</v>
+        <f>ROUND(D36*Computation!$B$34,0)</f>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -3318,15 +3337,15 @@
       </c>
       <c r="B39">
         <f>B36-B38</f>
-        <v>255</v>
+        <v>139</v>
       </c>
       <c r="C39">
         <f t="shared" ref="C39:D39" si="3">C36-C38</f>
-        <v>290</v>
+        <v>116</v>
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>217</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -3335,15 +3354,15 @@
       </c>
       <c r="B40">
         <f>ROUND(B37*Computation!$B$34,0)</f>
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="C40">
-        <f>ROUND(C37*Computation!$C$34,0)</f>
-        <v>0</v>
+        <f>ROUND(C37*Computation!$B$34,0)</f>
+        <v>296</v>
       </c>
       <c r="D40">
-        <f>ROUND(D37*Computation!$C$34,0)</f>
-        <v>0</v>
+        <f>ROUND(D37*Computation!$B$34,0)</f>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -3352,15 +3371,15 @@
       </c>
       <c r="B41">
         <f>B37-B40</f>
-        <v>433</v>
+        <v>237</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="4">C37-C40</f>
-        <v>493</v>
+        <v>197</v>
       </c>
       <c r="D41">
         <f t="shared" si="4"/>
-        <v>370</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -3422,119 +3441,119 @@
       <c r="A46" t="s">
         <v>84</v>
       </c>
-      <c r="B46" t="e">
-        <f>ROUND(B45*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C46" t="e">
-        <f>ROUND(C45*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D46" t="e">
-        <f>ROUND(D45*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
+      <c r="B46">
+        <f>ROUND(B45*'Static Data'!$B$2,0)</f>
+        <v>762</v>
+      </c>
+      <c r="C46">
+        <f>ROUND(C45*'Static Data'!$B$2,0)</f>
+        <v>635</v>
+      </c>
+      <c r="D46">
+        <f>ROUND(D45*'Static Data'!$B$2,0)</f>
+        <v>476</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>85</v>
       </c>
-      <c r="B47" t="e">
+      <c r="B47">
         <f>B45-B46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C47" t="e">
+        <v>1297</v>
+      </c>
+      <c r="C47">
         <f t="shared" ref="C47" si="6">C45-C46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D47" t="e">
+        <v>1081</v>
+      </c>
+      <c r="D47">
         <f t="shared" ref="D47" si="7">D45-D46</f>
-        <v>#REF!</v>
+        <v>811</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="e">
-        <f>ROUND(B46*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C48" t="e">
-        <f>ROUND(C46*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D48" t="e">
-        <f>ROUND(D46*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B48">
+        <f>ROUND(B46*Computation!$B$34,0)</f>
+        <v>457</v>
+      </c>
+      <c r="C48">
+        <f>ROUND(C46*Computation!$B$34,0)</f>
+        <v>381</v>
+      </c>
+      <c r="D48">
+        <f>ROUND(D46*Computation!$B$34,0)</f>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>87</v>
       </c>
-      <c r="B49" t="e">
+      <c r="B49">
         <f>B46-B48</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C49" t="e">
+        <v>305</v>
+      </c>
+      <c r="C49">
         <f t="shared" ref="C49" si="8">C46-C48</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D49" t="e">
+        <v>254</v>
+      </c>
+      <c r="D49">
         <f t="shared" ref="D49" si="9">D46-D48</f>
-        <v>#REF!</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B50" t="e">
-        <f>ROUND(B47*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C50" t="e">
-        <f>ROUND(C47*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D50" t="e">
-        <f>ROUND(D47*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B50">
+        <f>ROUND(B47*Computation!$B$34,0)</f>
+        <v>778</v>
+      </c>
+      <c r="C50">
+        <f>ROUND(C47*Computation!$B$34,0)</f>
+        <v>649</v>
+      </c>
+      <c r="D50">
+        <f>ROUND(D47*Computation!$B$34,0)</f>
+        <v>487</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>89</v>
       </c>
-      <c r="B51" t="e">
+      <c r="B51">
         <f>B47-B50</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C51" t="e">
+        <v>519</v>
+      </c>
+      <c r="C51">
         <f t="shared" ref="C51" si="10">C47-C50</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D51" t="e">
+        <v>432</v>
+      </c>
+      <c r="D51">
         <f t="shared" ref="D51" si="11">D47-D50</f>
-        <v>#REF!</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>90</v>
       </c>
-      <c r="B52" t="e">
+      <c r="B52">
         <f>SUM(B50:B51)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C52" t="e">
+        <v>1297</v>
+      </c>
+      <c r="C52">
         <f t="shared" ref="C52" si="12">SUM(C50:C51)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D52" t="e">
+        <v>1081</v>
+      </c>
+      <c r="D52">
         <f t="shared" ref="D52" si="13">SUM(D50:D51)</f>
-        <v>#REF!</v>
+        <v>811</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -3581,17 +3600,17 @@
       <c r="A56" t="s">
         <v>84</v>
       </c>
-      <c r="B56" t="e">
-        <f>ROUND(B55*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C56" t="e">
-        <f>ROUND(C55*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D56" t="e">
-        <f>ROUND(D55*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
+      <c r="B56">
+        <f>ROUND(B55*'Static Data'!$B$3,0)</f>
+        <v>1058</v>
+      </c>
+      <c r="C56">
+        <f>ROUND(C55*'Static Data'!$B$3,0)</f>
+        <v>881</v>
+      </c>
+      <c r="D56">
+        <f>ROUND(D55*'Static Data'!$B$3,0)</f>
+        <v>661</v>
       </c>
       <c r="F56" s="7"/>
     </row>
@@ -3599,17 +3618,17 @@
       <c r="A57" t="s">
         <v>85</v>
       </c>
-      <c r="B57" t="e">
+      <c r="B57">
         <f>B55-B56</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C57" t="e">
+        <v>676</v>
+      </c>
+      <c r="C57">
         <f t="shared" ref="C57" si="14">C55-C56</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D57" t="e">
+        <v>564</v>
+      </c>
+      <c r="D57">
         <f t="shared" ref="D57" si="15">D55-D56</f>
-        <v>#REF!</v>
+        <v>423</v>
       </c>
       <c r="F57" s="7"/>
     </row>
@@ -3617,17 +3636,17 @@
       <c r="A58" t="s">
         <v>86</v>
       </c>
-      <c r="B58" t="e">
-        <f>ROUND(B56*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C58" t="e">
-        <f>ROUND(C56*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D58" t="e">
-        <f>ROUND(D56*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B58">
+        <f>ROUND(B56*Computation!$B$34,0)</f>
+        <v>635</v>
+      </c>
+      <c r="C58">
+        <f>ROUND(C56*Computation!$B$34,0)</f>
+        <v>529</v>
+      </c>
+      <c r="D58">
+        <f>ROUND(D56*Computation!$B$34,0)</f>
+        <v>397</v>
       </c>
       <c r="F58" s="7"/>
     </row>
@@ -3635,17 +3654,17 @@
       <c r="A59" t="s">
         <v>87</v>
       </c>
-      <c r="B59" t="e">
+      <c r="B59">
         <f>B56-B58</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C59" t="e">
+        <v>423</v>
+      </c>
+      <c r="C59">
         <f t="shared" ref="C59" si="16">C56-C58</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D59" t="e">
+        <v>352</v>
+      </c>
+      <c r="D59">
         <f t="shared" ref="D59" si="17">D56-D58</f>
-        <v>#REF!</v>
+        <v>264</v>
       </c>
       <c r="F59" s="7"/>
     </row>
@@ -3653,51 +3672,51 @@
       <c r="A60" t="s">
         <v>88</v>
       </c>
-      <c r="B60" t="e">
-        <f>ROUND(B57*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C60" t="e">
-        <f>ROUND(C57*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D60" t="e">
-        <f>ROUND(D57*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B60">
+        <f>ROUND(B57*Computation!$B$34,0)</f>
+        <v>406</v>
+      </c>
+      <c r="C60">
+        <f>ROUND(C57*Computation!$B$34,0)</f>
+        <v>338</v>
+      </c>
+      <c r="D60">
+        <f>ROUND(D57*Computation!$B$34,0)</f>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>89</v>
       </c>
-      <c r="B61" t="e">
+      <c r="B61">
         <f>B57-B60</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C61" t="e">
+        <v>270</v>
+      </c>
+      <c r="C61">
         <f t="shared" ref="C61" si="18">C57-C60</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D61" t="e">
+        <v>226</v>
+      </c>
+      <c r="D61">
         <f t="shared" ref="D61" si="19">D57-D60</f>
-        <v>#REF!</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>90</v>
       </c>
-      <c r="B62" t="e">
+      <c r="B62">
         <f>SUM(B60:B61)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C62" t="e">
+        <v>676</v>
+      </c>
+      <c r="C62">
         <f t="shared" ref="C62" si="20">SUM(C60:C61)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D62" t="e">
+        <v>564</v>
+      </c>
+      <c r="D62">
         <f t="shared" ref="D62" si="21">SUM(D60:D61)</f>
-        <v>#REF!</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3742,119 +3761,119 @@
       <c r="A66" t="s">
         <v>84</v>
       </c>
-      <c r="B66" t="e">
-        <f>ROUND(B65*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C66" t="e">
-        <f>ROUND(C65*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D66" t="e">
-        <f>ROUND(D65*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
+      <c r="B66">
+        <f>ROUND(B65*'Static Data'!$B$4,0)</f>
+        <v>1245</v>
+      </c>
+      <c r="C66">
+        <f>ROUND(C65*'Static Data'!$B$4,0)</f>
+        <v>1038</v>
+      </c>
+      <c r="D66">
+        <f>ROUND(D65*'Static Data'!$B$4,0)</f>
+        <v>778</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>85</v>
       </c>
-      <c r="B67" t="e">
+      <c r="B67">
         <f>B65-B66</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C67" t="e">
+        <v>534</v>
+      </c>
+      <c r="C67">
         <f t="shared" ref="C67" si="22">C65-C66</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D67" t="e">
+        <v>445</v>
+      </c>
+      <c r="D67">
         <f t="shared" ref="D67" si="23">D65-D66</f>
-        <v>#REF!</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>86</v>
       </c>
-      <c r="B68" t="e">
-        <f>ROUND(B66*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C68" t="e">
-        <f>ROUND(C66*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D68" t="e">
-        <f>ROUND(D66*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B68">
+        <f>ROUND(B66*Computation!$B$34,0)</f>
+        <v>747</v>
+      </c>
+      <c r="C68">
+        <f>ROUND(C66*Computation!$B$34,0)</f>
+        <v>623</v>
+      </c>
+      <c r="D68">
+        <f>ROUND(D66*Computation!$B$34,0)</f>
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>87</v>
       </c>
-      <c r="B69" t="e">
+      <c r="B69">
         <f>B66-B68</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C69" t="e">
+        <v>498</v>
+      </c>
+      <c r="C69">
         <f t="shared" ref="C69" si="24">C66-C68</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D69" t="e">
+        <v>415</v>
+      </c>
+      <c r="D69">
         <f t="shared" ref="D69" si="25">D66-D68</f>
-        <v>#REF!</v>
+        <v>311</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
-      <c r="B70" t="e">
-        <f>ROUND(B67*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C70" t="e">
-        <f>ROUND(C67*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D70" t="e">
-        <f>ROUND(D67*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B70">
+        <f>ROUND(B67*Computation!$B$34,0)</f>
+        <v>320</v>
+      </c>
+      <c r="C70">
+        <f>ROUND(C67*Computation!$B$34,0)</f>
+        <v>267</v>
+      </c>
+      <c r="D70">
+        <f>ROUND(D67*Computation!$B$34,0)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>89</v>
       </c>
-      <c r="B71" t="e">
+      <c r="B71">
         <f>B67-B70</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C71" t="e">
+        <v>214</v>
+      </c>
+      <c r="C71">
         <f t="shared" ref="C71" si="26">C67-C70</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D71" t="e">
+        <v>178</v>
+      </c>
+      <c r="D71">
         <f t="shared" ref="D71" si="27">D67-D70</f>
-        <v>#REF!</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>90</v>
       </c>
-      <c r="B72" t="e">
+      <c r="B72">
         <f>SUM(B70:B71)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C72" t="e">
+        <v>534</v>
+      </c>
+      <c r="C72">
         <f t="shared" ref="C72" si="28">SUM(C70:C71)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D72" t="e">
+        <v>445</v>
+      </c>
+      <c r="D72">
         <f t="shared" ref="D72" si="29">SUM(D70:D71)</f>
-        <v>#REF!</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -3899,119 +3918,119 @@
       <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B76" t="e">
-        <f>ROUND(B75*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C76" t="e">
-        <f>ROUND(C75*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D76" t="e">
-        <f>ROUND(D75*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
+      <c r="B76">
+        <f>ROUND(B75*'Static Data'!$B$5,0)</f>
+        <v>985</v>
+      </c>
+      <c r="C76">
+        <f>ROUND(C75*'Static Data'!$B$5,0)</f>
+        <v>821</v>
+      </c>
+      <c r="D76">
+        <f>ROUND(D75*'Static Data'!$B$5,0)</f>
+        <v>616</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>85</v>
       </c>
-      <c r="B77" t="e">
+      <c r="B77">
         <f>B75-B76</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C77" t="e">
+        <v>311</v>
+      </c>
+      <c r="C77">
         <f t="shared" ref="C77" si="30">C75-C76</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D77" t="e">
+        <v>259</v>
+      </c>
+      <c r="D77">
         <f t="shared" ref="D77" si="31">D75-D76</f>
-        <v>#REF!</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>86</v>
       </c>
-      <c r="B78" t="e">
-        <f>ROUND(B76*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C78" t="e">
-        <f>ROUND(C76*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D78" t="e">
-        <f>ROUND(D76*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B78">
+        <f>ROUND(B76*Computation!$B$34,0)</f>
+        <v>591</v>
+      </c>
+      <c r="C78">
+        <f>ROUND(C76*Computation!$B$34,0)</f>
+        <v>493</v>
+      </c>
+      <c r="D78">
+        <f>ROUND(D76*Computation!$B$34,0)</f>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>87</v>
       </c>
-      <c r="B79" t="e">
+      <c r="B79">
         <f>B76-B78</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C79" t="e">
+        <v>394</v>
+      </c>
+      <c r="C79">
         <f t="shared" ref="C79" si="32">C76-C78</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D79" t="e">
+        <v>328</v>
+      </c>
+      <c r="D79">
         <f t="shared" ref="D79" si="33">D76-D78</f>
-        <v>#REF!</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>88</v>
       </c>
-      <c r="B80" t="e">
-        <f>ROUND(B77*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C80" t="e">
-        <f>ROUND(C77*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D80" t="e">
-        <f>ROUND(D77*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B80">
+        <f>ROUND(B77*Computation!$B$34,0)</f>
+        <v>187</v>
+      </c>
+      <c r="C80">
+        <f>ROUND(C77*Computation!$B$34,0)</f>
+        <v>155</v>
+      </c>
+      <c r="D80">
+        <f>ROUND(D77*Computation!$B$34,0)</f>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>89</v>
       </c>
-      <c r="B81" t="e">
+      <c r="B81">
         <f>B77-B80</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C81" t="e">
+        <v>124</v>
+      </c>
+      <c r="C81">
         <f t="shared" ref="C81" si="34">C77-C80</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D81" t="e">
+        <v>104</v>
+      </c>
+      <c r="D81">
         <f t="shared" ref="D81" si="35">D77-D80</f>
-        <v>#REF!</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>90</v>
       </c>
-      <c r="B82" t="e">
+      <c r="B82">
         <f>SUM(B80:B81)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C82" t="e">
+        <v>311</v>
+      </c>
+      <c r="C82">
         <f t="shared" ref="C82" si="36">SUM(C80:C81)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D82" t="e">
+        <v>259</v>
+      </c>
+      <c r="D82">
         <f t="shared" ref="D82" si="37">SUM(D80:D81)</f>
-        <v>#REF!</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -4056,119 +4075,119 @@
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86" t="e">
-        <f>ROUND(B85*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C86" t="e">
-        <f>ROUND(C85*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D86" t="e">
-        <f>ROUND(D85*'Sample Zip Data'!#REF!,0)</f>
-        <v>#REF!</v>
+      <c r="B86">
+        <f>ROUND(B85*'Static Data'!$B$6,0)</f>
+        <v>1125</v>
+      </c>
+      <c r="C86">
+        <f>ROUND(C85*'Static Data'!$B$6,0)</f>
+        <v>938</v>
+      </c>
+      <c r="D86">
+        <f>ROUND(D85*'Static Data'!$B$6,0)</f>
+        <v>703</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" t="e">
+      <c r="B87">
         <f>B85-B86</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C87" t="e">
+        <v>299</v>
+      </c>
+      <c r="C87">
         <f t="shared" ref="C87" si="38">C85-C86</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D87" t="e">
+        <v>249</v>
+      </c>
+      <c r="D87">
         <f t="shared" ref="D87" si="39">D85-D86</f>
-        <v>#REF!</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" t="e">
-        <f>ROUND(B86*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C88" t="e">
-        <f>ROUND(C86*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D88" t="e">
-        <f>ROUND(D86*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B88">
+        <f>ROUND(B86*Computation!$B$34,0)</f>
+        <v>675</v>
+      </c>
+      <c r="C88">
+        <f>ROUND(C86*Computation!$B$34,0)</f>
+        <v>563</v>
+      </c>
+      <c r="D88">
+        <f>ROUND(D86*Computation!$B$34,0)</f>
+        <v>422</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" t="e">
+      <c r="B89">
         <f>B86-B88</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C89" t="e">
+        <v>450</v>
+      </c>
+      <c r="C89">
         <f t="shared" ref="C89" si="40">C86-C88</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D89" t="e">
+        <v>375</v>
+      </c>
+      <c r="D89">
         <f t="shared" ref="D89" si="41">D86-D88</f>
-        <v>#REF!</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90" t="e">
-        <f>ROUND(B87*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C90" t="e">
-        <f>ROUND(C87*Computation!$C$34,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D90" t="e">
-        <f>ROUND(D87*Computation!$C$34,0)</f>
-        <v>#REF!</v>
+      <c r="B90">
+        <f>ROUND(B87*Computation!$B$34,0)</f>
+        <v>179</v>
+      </c>
+      <c r="C90">
+        <f>ROUND(C87*Computation!$B$34,0)</f>
+        <v>149</v>
+      </c>
+      <c r="D90">
+        <f>ROUND(D87*Computation!$B$34,0)</f>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91" t="e">
+      <c r="B91">
         <f>B87-B90</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C91" t="e">
+        <v>120</v>
+      </c>
+      <c r="C91">
         <f t="shared" ref="C91" si="42">C87-C90</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D91" t="e">
+        <v>100</v>
+      </c>
+      <c r="D91">
         <f t="shared" ref="D91" si="43">D87-D90</f>
-        <v>#REF!</v>
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" t="e">
+      <c r="B92">
         <f>SUM(B90:B91)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C92" t="e">
+        <v>299</v>
+      </c>
+      <c r="C92">
         <f t="shared" ref="C92" si="44">SUM(C90:C91)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D92" t="e">
+        <v>249</v>
+      </c>
+      <c r="D92">
         <f t="shared" ref="D92" si="45">SUM(D90:D91)</f>
-        <v>#REF!</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -4199,7 +4218,7 @@
         <f>B42</f>
         <v>592</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="23">
         <v>1542</v>
       </c>
       <c r="D95" s="1">
@@ -4215,107 +4234,107 @@
       <c r="A96" t="s">
         <v>7</v>
       </c>
-      <c r="B96" t="e">
+      <c r="B96">
         <f>B52</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C96">
+        <v>1297</v>
+      </c>
+      <c r="C96" s="23">
         <v>920</v>
       </c>
       <c r="D96" s="1">
         <f>Computation!E22</f>
         <v>3.7936772046589018E-2</v>
       </c>
-      <c r="E96" t="e">
+      <c r="E96">
         <f t="shared" ref="E96:E100" si="46">ROUND(B96*(1+D96),0)</f>
-        <v>#REF!</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" t="e">
+      <c r="B97">
         <f>B62</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C97">
+        <v>676</v>
+      </c>
+      <c r="C97" s="23">
         <v>909</v>
       </c>
       <c r="D97" s="1">
         <f>Computation!E23</f>
         <v>3.795966785290629E-2</v>
       </c>
-      <c r="E97" t="e">
+      <c r="E97">
         <f t="shared" si="46"/>
-        <v>#REF!</v>
+        <v>702</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" t="e">
+      <c r="B98">
         <f>B72</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C98">
+        <v>534</v>
+      </c>
+      <c r="C98" s="23">
         <v>876</v>
       </c>
       <c r="D98" s="1">
         <f>Computation!E24</f>
         <v>-2.0712510356255178E-2</v>
       </c>
-      <c r="E98" t="e">
+      <c r="E98">
         <f t="shared" si="46"/>
-        <v>#REF!</v>
+        <v>523</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
-      <c r="B99" t="e">
+      <c r="B99">
         <f>B82</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C99">
+        <v>311</v>
+      </c>
+      <c r="C99" s="23">
         <v>641</v>
       </c>
       <c r="D99" s="1">
         <f>Computation!E25</f>
         <v>-2.1034678794769755E-2</v>
       </c>
-      <c r="E99" t="e">
+      <c r="E99">
         <f t="shared" si="46"/>
-        <v>#REF!</v>
+        <v>304</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>
-      <c r="B100" t="e">
+      <c r="B100">
         <f>B92</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C100">
+        <v>299</v>
+      </c>
+      <c r="C100" s="23">
         <v>618</v>
       </c>
       <c r="D100" s="1">
         <f>Computation!E26</f>
         <v>0.12494632889652212</v>
       </c>
-      <c r="E100" t="e">
+      <c r="E100">
         <f t="shared" si="46"/>
-        <v>#REF!</v>
+        <v>336</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="22">
         <v>2024</v>
       </c>
     </row>
@@ -4323,7 +4342,7 @@
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="23">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made some fixes to the tam exporter and tam template
</commit_message>
<xml_diff>
--- a/xls/templates/tam-template.xlsx
+++ b/xls/templates/tam-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BC3FC3-8856-E447-9627-3CAB3A8AB5F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E42E1E-4C66-5A4A-8FBF-12F0E42DFF24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="460" windowWidth="33260" windowHeight="20440" activeTab="2" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33260" windowHeight="20440" activeTab="2" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Zip Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
   <si>
     <t>Rent Stats</t>
   </si>
@@ -186,9 +186,6 @@
     <t>20th</t>
   </si>
   <si>
-    <t>RTI Pop Growth by Year</t>
-  </si>
-  <si>
     <t>Market Growth Until 2023</t>
   </si>
   <si>
@@ -379,6 +376,15 @@
   </si>
   <si>
     <t>Total Population</t>
+  </si>
+  <si>
+    <t>Seg %</t>
+  </si>
+  <si>
+    <t>Seg Count</t>
+  </si>
+  <si>
+    <t>Pop Total</t>
   </si>
 </sst>
 </file>
@@ -524,7 +530,6 @@
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -532,7 +537,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,12 +554,16 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="9" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="6"/>
-    <xf numFmtId="9" fontId="11" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -878,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E632269-A679-4E49-9C55-0C6771CDB655}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,50 +902,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="17">
         <v>950</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="17">
         <v>750</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>778</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>21371</v>
       </c>
     </row>
@@ -1038,10 +1046,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="8"/>
       <c r="E16" t="s">
         <v>18</v>
       </c>
@@ -1171,7 +1179,7 @@
       <c r="C27" s="1">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1232,56 +1240,56 @@
       <c r="D32" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>0.18323353000000001</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>4.5109780000000002E-2</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>4.0319359999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>0.57325349000000003</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>0.15808383000000001</v>
       </c>
     </row>
@@ -1290,7 +1298,7 @@
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
@@ -1301,7 +1309,7 @@
       <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="13">
         <v>235200</v>
       </c>
       <c r="C42" s="1"/>
@@ -1311,7 +1319,7 @@
       <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="13">
         <v>105300</v>
       </c>
     </row>
@@ -1319,7 +1327,7 @@
       <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="13">
         <v>63400</v>
       </c>
       <c r="C44" s="1"/>
@@ -1329,7 +1337,7 @@
       <c r="A45" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="13">
         <v>50200</v>
       </c>
       <c r="C45" s="1"/>
@@ -1339,7 +1347,7 @@
       <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="13">
         <v>40800</v>
       </c>
     </row>
@@ -1347,7 +1355,7 @@
       <c r="A47" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="13">
         <v>21000</v>
       </c>
       <c r="C47" s="1"/>
@@ -1372,7 +1380,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,36 +1435,36 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
         <v>105</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>107</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>108</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>109</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>110</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>111</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>112</v>
-      </c>
-      <c r="I9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1640,57 +1648,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059DB5A-4215-0640-95EF-B3BB098332D1}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3">
         <v>2016</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>2017</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>2018</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>2019</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>2020</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>2021</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>2022</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>2023</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>2024</v>
       </c>
     </row>
@@ -1698,7 +1706,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="23">
         <f>ROUND('Sample Zip Data'!B8*(1+'Static Data'!B10),0)</f>
         <v>1827</v>
       </c>
@@ -1739,7 +1747,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="23">
         <f>ROUND('Sample Zip Data'!B9*(1+'Static Data'!B11),0)</f>
         <v>3893</v>
       </c>
@@ -1780,7 +1788,7 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="23">
         <f>ROUND('Sample Zip Data'!B10*(1+'Static Data'!B12),0)</f>
         <v>3276</v>
       </c>
@@ -1821,7 +1829,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="23">
         <f>ROUND('Sample Zip Data'!B11*(1+'Static Data'!B13),0)</f>
         <v>3449</v>
       </c>
@@ -1862,7 +1870,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="23">
         <f>ROUND('Sample Zip Data'!B12*(1+'Static Data'!B14),0)</f>
         <v>2512</v>
       </c>
@@ -1903,7 +1911,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="23">
         <f>ROUND('Sample Zip Data'!B13*(1+'Static Data'!B15),0)</f>
         <v>2587</v>
       </c>
@@ -1941,517 +1949,253 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4">
-        <v>2016</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2017</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2018</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="B11">
         <v>2019</v>
       </c>
-      <c r="F11" s="4">
-        <v>2020</v>
-      </c>
-      <c r="G11" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H11" s="4">
-        <v>2022</v>
-      </c>
-      <c r="I11" s="4">
-        <v>2023</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="C11">
         <v>2024</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="26">
-        <f>ROUND(B3*SUM($B$29:$B$31),0)</f>
-        <v>1315</v>
+      <c r="B12">
+        <f>E3</f>
+        <v>1806</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:J12" si="0">ROUND(C3*SUM($B$29:$B$31),0)</f>
-        <v>1310</v>
+        <f>I3</f>
+        <v>1808</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1305</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1300</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>1295</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>1297</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>1300</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>1302</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>1304</v>
+        <f>C12-B12</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <f>D12/C12</f>
+        <v>1.1061946902654867E-3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="26">
-        <f t="shared" ref="B13:J17" si="1">ROUND(B4*SUM($B$29:$B$31),0)</f>
-        <v>2803</v>
+      <c r="B13">
+        <f t="shared" ref="B13:B17" si="0">E4</f>
+        <v>4015</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>2832</v>
+        <f t="shared" ref="C13:C17" si="1">I4</f>
+        <v>4173</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>2861</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>2891</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>2921</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>2948</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>2976</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>3005</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>3033</v>
+        <f t="shared" ref="D13:D17" si="2">C13-B13</f>
+        <v>158</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ref="E13:E17" si="3">D13/C13</f>
+        <v>3.7862449077402348E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="26">
-        <f t="shared" si="1"/>
-        <v>2359</v>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>3379</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>2383</v>
+        <v>3512</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>2408</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>2433</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>2458</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
-        <v>2481</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>2505</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>2529</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>2552</v>
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7870159453302958E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="26">
-        <f t="shared" si="1"/>
-        <v>2483</v>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>3422</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>2477</v>
+        <v>3353</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>2470</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>2464</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>2457</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>2443</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>2429</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>2414</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>2400</v>
+        <f t="shared" si="2"/>
+        <v>-69</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.0578586340590517E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="26">
-        <f t="shared" si="1"/>
-        <v>1809</v>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>2494</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>1804</v>
+        <v>2443</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>1800</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>1796</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>1791</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="1"/>
-        <v>1781</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>1770</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>1759</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>-51</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.0875972165370446E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="26">
-        <f t="shared" si="1"/>
-        <v>1863</v>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2830</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>1920</v>
+        <v>3235</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>1978</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>2038</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>2100</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>2174</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>2250</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>2329</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>2411</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>2019</v>
-      </c>
-      <c r="C20">
-        <v>2024</v>
-      </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" t="s">
+        <f t="shared" si="2"/>
+        <v>405</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="3"/>
+        <v>0.12519319938176199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <f>E12</f>
-        <v>1300</v>
-      </c>
-      <c r="C21">
-        <f>I12</f>
-        <v>1302</v>
-      </c>
-      <c r="D21">
-        <f>C21-B21</f>
-        <v>2</v>
-      </c>
-      <c r="E21" s="6">
-        <f>D21/C21</f>
-        <v>1.5360983102918587E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <f t="shared" ref="B22:B26" si="2">E13</f>
-        <v>2891</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:C26" si="3">I13</f>
-        <v>3005</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22:D26" si="4">C22-B22</f>
+      <c r="B19" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="6">
-        <f t="shared" ref="E22:E26" si="5">D22/C22</f>
-        <v>3.7936772046589018E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="2"/>
-        <v>2433</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="3"/>
-        <v>2529</v>
-      </c>
-      <c r="D23">
+      <c r="C19" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="25">
+        <v>25000</v>
+      </c>
+      <c r="B20" s="24">
+        <f>C20/D20</f>
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="25">
+        <v>35000</v>
+      </c>
+      <c r="B21" s="24">
+        <f t="shared" ref="B21:B22" si="4">C21/D21</f>
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="25">
+        <v>45000</v>
+      </c>
+      <c r="B22" s="24">
         <f t="shared" si="4"/>
-        <v>96</v>
-      </c>
-      <c r="E23" s="6">
-        <f t="shared" si="5"/>
-        <v>3.795966785290629E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="2"/>
-        <v>2464</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="3"/>
-        <v>2414</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="4"/>
-        <v>-50</v>
-      </c>
-      <c r="E24" s="6">
-        <f t="shared" si="5"/>
-        <v>-2.0712510356255178E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>100</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="2"/>
-        <v>1796</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="3"/>
-        <v>1759</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="4"/>
-        <v>-37</v>
-      </c>
-      <c r="E25" s="6">
-        <f t="shared" si="5"/>
-        <v>-2.1034678794769755E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="2"/>
-        <v>2038</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="3"/>
-        <v>2329</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="4"/>
-        <v>291</v>
-      </c>
-      <c r="E26" s="6">
-        <f t="shared" si="5"/>
-        <v>0.12494632889652212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>25000</v>
-      </c>
-      <c r="B29" s="27">
-        <v>0.12</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>35000</v>
-      </c>
-      <c r="B30" s="27">
-        <v>0.15</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="8">
-        <v>45000</v>
-      </c>
-      <c r="B31" s="27">
-        <v>0.45</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="17"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B26" s="4">
+        <f>1-B25</f>
+        <v>0.4</v>
+      </c>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5">
-        <f>1-B34</f>
-        <v>0.4</v>
-      </c>
-      <c r="C35" s="16"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="5">
-        <f>SUM(B34:B35)</f>
+      <c r="B27" s="4">
+        <f>SUM(B25:B26)</f>
         <v>1</v>
       </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="26">
+      <c r="C27" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="23">
         <v>10000</v>
       </c>
     </row>
@@ -2465,245 +2209,245 @@
   <dimension ref="A1:Q104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>59</v>
+      <c r="A1" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="23">
+        <v>61</v>
+      </c>
+      <c r="B3" s="21">
         <v>33.484937100000003</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="21">
         <v>-112.0856505</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="23">
+        <v>62</v>
+      </c>
+      <c r="B4" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="2">
+        <f>Computation!B29</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="3">
-        <f>Computation!B38</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="2">
+        <f>SUM(B95:B100)</f>
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="3">
-        <f>SUM(B95:B100)</f>
-        <v>3709</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <f>SUM(C95:C100)</f>
         <v>5506</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="2">
+        <f>SUM(E95:E100)</f>
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="3">
-        <f>SUM(E95:E100)</f>
-        <v>3804</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="22">
+        <v>750</v>
+      </c>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="22">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="25">
-        <v>950</v>
-      </c>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="25">
-        <v>750</v>
-      </c>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="25">
-        <f>'Sample Zip Data'!B4</f>
-        <v>778</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="22">
+        <v>74</v>
+      </c>
+      <c r="B18" s="20">
         <v>0</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="20">
         <v>0.12</v>
       </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="22">
+        <v>75</v>
+      </c>
+      <c r="B19" s="20">
         <v>0.12</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="20">
         <v>0.24</v>
       </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="22">
+        <v>76</v>
+      </c>
+      <c r="B20" s="20">
         <v>0.24</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="20">
         <v>0.35</v>
       </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="22">
+        <v>77</v>
+      </c>
+      <c r="B21" s="20">
         <v>0.35</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="20">
         <v>0.45</v>
       </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="C22" s="20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B22" s="22">
-        <v>0.45</v>
-      </c>
-      <c r="C22" s="22">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="B23">
         <v>15000</v>
@@ -2738,520 +2482,523 @@
       <c r="L23">
         <v>65000</v>
       </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>500</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <f>$A24/(B$23/12)</f>
         <v>0.4</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <f t="shared" ref="C24:L24" si="0">$A24/(C$23/12)</f>
         <v>0.3</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <f t="shared" si="0"/>
         <v>0.17142857142857143</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <f t="shared" si="0"/>
         <v>0.1090909090909091</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="4">
         <f t="shared" si="0"/>
         <v>9.2307692307692299E-2</v>
       </c>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>600</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <f t="shared" ref="B25:L32" si="1">$A25/(B$23/12)</f>
         <v>0.48</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <f t="shared" si="1"/>
         <v>0.28799999999999998</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <f t="shared" si="1"/>
         <v>0.20571428571428574</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="4">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <f t="shared" si="1"/>
         <v>0.14399999999999999</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4">
         <f t="shared" si="1"/>
         <v>0.13090909090909092</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="4">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="4">
         <f t="shared" si="1"/>
         <v>0.11076923076923076</v>
       </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>700</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <f t="shared" si="1"/>
         <v>0.33599999999999997</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <f t="shared" si="1"/>
         <v>0.24000000000000002</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <f t="shared" si="1"/>
         <v>0.21</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <f t="shared" si="1"/>
         <v>0.18666666666666668</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <f t="shared" si="1"/>
         <v>0.16799999999999998</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="4">
         <f t="shared" si="1"/>
         <v>0.15272727272727274</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="4">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26" s="4">
         <f t="shared" si="1"/>
         <v>0.12923076923076923</v>
       </c>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>800</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <f t="shared" si="1"/>
         <v>0.38399999999999995</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <f t="shared" si="1"/>
         <v>0.2742857142857143</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="4">
         <f t="shared" si="1"/>
         <v>0.21333333333333335</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="4">
         <f t="shared" si="1"/>
         <v>0.19199999999999998</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="4">
         <f t="shared" si="1"/>
         <v>0.17454545454545456</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="4">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L27" s="4">
         <f t="shared" si="1"/>
         <v>0.14769230769230768</v>
       </c>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>900</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <f t="shared" si="1"/>
         <v>0.53999999999999992</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f t="shared" si="1"/>
         <v>0.432</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <f t="shared" si="1"/>
         <v>0.30857142857142861</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <f t="shared" si="1"/>
         <v>0.26999999999999996</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="4">
         <f t="shared" si="1"/>
         <v>0.216</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="4">
         <f t="shared" si="1"/>
         <v>0.19636363636363638</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="4">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="4">
         <f t="shared" si="1"/>
         <v>0.16615384615384615</v>
       </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1000</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <f t="shared" si="1"/>
         <v>0.34285714285714286</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="4">
         <f t="shared" si="1"/>
         <v>0.2181818181818182</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="4">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L29" s="5">
+      <c r="L29" s="4">
         <f t="shared" si="1"/>
         <v>0.1846153846153846</v>
       </c>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1100</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <f t="shared" si="1"/>
         <v>0.88</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <f t="shared" si="1"/>
         <v>0.65999999999999992</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <f t="shared" si="1"/>
         <v>0.52799999999999991</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="4">
         <f t="shared" si="1"/>
         <v>0.37714285714285717</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <f t="shared" si="1"/>
         <v>0.32999999999999996</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="4">
         <f t="shared" si="1"/>
         <v>0.29333333333333333</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="4">
         <f t="shared" si="1"/>
         <v>0.26399999999999996</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4">
         <f t="shared" si="1"/>
         <v>0.24000000000000002</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="4">
         <f t="shared" si="1"/>
         <v>0.22</v>
       </c>
-      <c r="L30" s="5">
+      <c r="L30" s="4">
         <f t="shared" si="1"/>
         <v>0.20307692307692307</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1200</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <f t="shared" si="1"/>
         <v>0.57599999999999996</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <f t="shared" si="1"/>
         <v>0.41142857142857148</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="4">
         <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="4">
         <f t="shared" si="1"/>
         <v>0.28799999999999998</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="4">
         <f t="shared" si="1"/>
         <v>0.26181818181818184</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="L31" s="5">
+      <c r="L31" s="4">
         <f t="shared" si="1"/>
         <v>0.22153846153846152</v>
       </c>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1300</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <f t="shared" si="1"/>
         <v>1.04</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <f t="shared" si="1"/>
         <v>0.77999999999999992</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <f t="shared" si="1"/>
         <v>0.624</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <f t="shared" si="1"/>
         <v>0.44571428571428573</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <f t="shared" si="1"/>
         <v>0.38999999999999996</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="4">
         <f t="shared" si="1"/>
         <v>0.34666666666666668</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="4">
         <f t="shared" si="1"/>
         <v>0.312</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="4">
         <f t="shared" si="1"/>
         <v>0.28363636363636363</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="4">
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
-      <c r="L32" s="5">
+      <c r="L32" s="4">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="26">
+        <f>Computation!$A$20</f>
+        <v>25000</v>
+      </c>
+      <c r="C34" s="26">
+        <f>Computation!$A$21</f>
+        <v>35000</v>
+      </c>
+      <c r="D34" s="26">
+        <f>Computation!$A$22</f>
+        <v>45000</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="18">
-        <v>25000</v>
-      </c>
-      <c r="C34" s="18">
-        <v>35000</v>
-      </c>
-      <c r="D34" s="18">
-        <v>45000</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="M34"/>
       <c r="N34"/>
@@ -3261,953 +3008,968 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35">
-        <f>ROUND(Computation!$D$12*Computation!B29,0)+C35</f>
-        <v>940</v>
+        <f>ROUND(E35*Computation!B20,0)+C35</f>
+        <v>543</v>
       </c>
       <c r="C35">
-        <f>ROUND(Computation!$D$12*Computation!B30,0)+D35</f>
-        <v>783</v>
+        <f>ROUND(E35*Computation!B21,0)+D35</f>
+        <v>362</v>
       </c>
       <c r="D35">
-        <f>ROUND(Computation!$D$12*Computation!B31,0)</f>
-        <v>587</v>
+        <f>ROUND(E35*Computation!B22,0)</f>
+        <v>181</v>
       </c>
       <c r="E35">
-        <f>ROUND(Computation!$D$12,0)</f>
-        <v>1305</v>
+        <f>ROUND(Computation!$E$3,0)</f>
+        <v>1806</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36">
         <f>ROUND(B35*'Static Data'!$B$2,0)</f>
-        <v>348</v>
+        <v>201</v>
       </c>
       <c r="C36">
         <f>ROUND(C35*'Static Data'!$B$2,0)</f>
-        <v>290</v>
+        <v>134</v>
       </c>
       <c r="D36">
         <f>ROUND(D35*'Static Data'!$B$2,0)</f>
-        <v>217</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37">
         <f>B35-B36</f>
-        <v>592</v>
+        <v>342</v>
       </c>
       <c r="C37">
         <f t="shared" ref="C37:D37" si="2">C35-C36</f>
-        <v>493</v>
+        <v>228</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>370</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38">
-        <f>ROUND(B36*Computation!$B$34,0)</f>
-        <v>209</v>
+        <f>ROUND(B36*Computation!$B$25,0)</f>
+        <v>121</v>
       </c>
       <c r="C38">
-        <f>ROUND(C36*Computation!$B$34,0)</f>
-        <v>174</v>
+        <f>ROUND(C36*Computation!$B$25,0)</f>
+        <v>80</v>
       </c>
       <c r="D38">
-        <f>ROUND(D36*Computation!$B$34,0)</f>
-        <v>130</v>
+        <f>ROUND(D36*Computation!$B$25,0)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39">
         <f>B36-B38</f>
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="C39">
         <f t="shared" ref="C39:D39" si="3">C36-C38</f>
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40">
-        <f>ROUND(B37*Computation!$B$34,0)</f>
-        <v>355</v>
+        <f>ROUND(B37*Computation!$B$25,0)</f>
+        <v>205</v>
       </c>
       <c r="C40">
-        <f>ROUND(C37*Computation!$B$34,0)</f>
-        <v>296</v>
+        <f>ROUND(C37*Computation!$B$25,0)</f>
+        <v>137</v>
       </c>
       <c r="D40">
-        <f>ROUND(D37*Computation!$B$34,0)</f>
-        <v>222</v>
+        <f>ROUND(D37*Computation!$B$25,0)</f>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41">
         <f>B37-B40</f>
-        <v>237</v>
+        <v>137</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:D41" si="4">C37-C40</f>
-        <v>197</v>
+        <v>91</v>
       </c>
       <c r="D41">
         <f t="shared" si="4"/>
-        <v>148</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42">
         <f>SUM(B40:B41)</f>
-        <v>592</v>
+        <v>342</v>
       </c>
       <c r="C42">
         <f t="shared" ref="C42:D42" si="5">SUM(C40:C41)</f>
-        <v>493</v>
+        <v>228</v>
       </c>
       <c r="D42">
         <f t="shared" si="5"/>
-        <v>370</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="18">
+      <c r="A44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="26">
+        <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="26">
+        <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="26">
+        <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>82</v>
+      <c r="E44" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45">
-        <f>ROUND(Computation!$D$13*Computation!B29,0)+C45</f>
-        <v>2059</v>
+        <f>ROUND(E45*Computation!B20,0)+C45</f>
+        <v>1206</v>
       </c>
       <c r="C45">
-        <f>ROUND(Computation!$D$13*Computation!B30,0)+D45</f>
-        <v>1716</v>
+        <f>ROUND(E45*Computation!B21,0)+D45</f>
+        <v>804</v>
       </c>
       <c r="D45">
-        <f>ROUND(Computation!$D$13*Computation!B31,0)</f>
-        <v>1287</v>
+        <f>ROUND(E45*Computation!B22,0)</f>
+        <v>402</v>
       </c>
       <c r="E45">
-        <f>ROUND(Computation!$D$13,0)</f>
-        <v>2861</v>
+        <f>ROUND(Computation!$E$4,0)</f>
+        <v>4015</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46">
         <f>ROUND(B45*'Static Data'!$B$2,0)</f>
-        <v>762</v>
+        <v>446</v>
       </c>
       <c r="C46">
         <f>ROUND(C45*'Static Data'!$B$2,0)</f>
-        <v>635</v>
+        <v>297</v>
       </c>
       <c r="D46">
         <f>ROUND(D45*'Static Data'!$B$2,0)</f>
-        <v>476</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47">
         <f>B45-B46</f>
-        <v>1297</v>
+        <v>760</v>
       </c>
       <c r="C47">
         <f t="shared" ref="C47" si="6">C45-C46</f>
-        <v>1081</v>
+        <v>507</v>
       </c>
       <c r="D47">
         <f t="shared" ref="D47" si="7">D45-D46</f>
-        <v>811</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48">
-        <f>ROUND(B46*Computation!$B$34,0)</f>
-        <v>457</v>
+        <f>ROUND(B46*Computation!$B$25,0)</f>
+        <v>268</v>
       </c>
       <c r="C48">
-        <f>ROUND(C46*Computation!$B$34,0)</f>
-        <v>381</v>
+        <f>ROUND(C46*Computation!$B$25,0)</f>
+        <v>178</v>
       </c>
       <c r="D48">
-        <f>ROUND(D46*Computation!$B$34,0)</f>
-        <v>286</v>
+        <f>ROUND(D46*Computation!$B$25,0)</f>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49">
         <f>B46-B48</f>
-        <v>305</v>
+        <v>178</v>
       </c>
       <c r="C49">
         <f t="shared" ref="C49" si="8">C46-C48</f>
-        <v>254</v>
+        <v>119</v>
       </c>
       <c r="D49">
         <f t="shared" ref="D49" si="9">D46-D48</f>
-        <v>190</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50">
-        <f>ROUND(B47*Computation!$B$34,0)</f>
-        <v>778</v>
+        <f>ROUND(B47*Computation!$B$25,0)</f>
+        <v>456</v>
       </c>
       <c r="C50">
-        <f>ROUND(C47*Computation!$B$34,0)</f>
-        <v>649</v>
+        <f>ROUND(C47*Computation!$B$25,0)</f>
+        <v>304</v>
       </c>
       <c r="D50">
-        <f>ROUND(D47*Computation!$B$34,0)</f>
-        <v>487</v>
+        <f>ROUND(D47*Computation!$B$25,0)</f>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51">
         <f>B47-B50</f>
-        <v>519</v>
+        <v>304</v>
       </c>
       <c r="C51">
         <f t="shared" ref="C51" si="10">C47-C50</f>
-        <v>432</v>
+        <v>203</v>
       </c>
       <c r="D51">
         <f t="shared" ref="D51" si="11">D47-D50</f>
-        <v>324</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52">
         <f>SUM(B50:B51)</f>
-        <v>1297</v>
+        <v>760</v>
       </c>
       <c r="C52">
         <f t="shared" ref="C52" si="12">SUM(C50:C51)</f>
-        <v>1081</v>
+        <v>507</v>
       </c>
       <c r="D52">
         <f t="shared" ref="D52" si="13">SUM(D50:D51)</f>
-        <v>811</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="18">
+      <c r="A54" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="26">
+        <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="26">
+        <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D54" s="18">
+      <c r="D54" s="26">
+        <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E54" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F54" s="7"/>
+      <c r="E54" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55">
-        <f>ROUND(Computation!$D$14*Computation!B29,0)+C55</f>
-        <v>1734</v>
+        <f>ROUND(E55*Computation!B20,0)+C55</f>
+        <v>1014</v>
       </c>
       <c r="C55">
-        <f>ROUND(Computation!$D$14*Computation!B30,0)+D55</f>
-        <v>1445</v>
+        <f>ROUND(E55*Computation!B21,0)+D55</f>
+        <v>676</v>
       </c>
       <c r="D55">
-        <f>ROUND(Computation!$D$14*Computation!B31,0)</f>
-        <v>1084</v>
+        <f>ROUND(E55*Computation!B22,0)</f>
+        <v>338</v>
       </c>
       <c r="E55">
-        <f>ROUND(Computation!$D$14,0)</f>
-        <v>2408</v>
-      </c>
-      <c r="F55" s="7"/>
+        <f>ROUND(Computation!$E$5,0)</f>
+        <v>3379</v>
+      </c>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56">
         <f>ROUND(B55*'Static Data'!$B$3,0)</f>
-        <v>1058</v>
+        <v>619</v>
       </c>
       <c r="C56">
         <f>ROUND(C55*'Static Data'!$B$3,0)</f>
-        <v>881</v>
+        <v>412</v>
       </c>
       <c r="D56">
         <f>ROUND(D55*'Static Data'!$B$3,0)</f>
-        <v>661</v>
-      </c>
-      <c r="F56" s="7"/>
+        <v>206</v>
+      </c>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57">
         <f>B55-B56</f>
-        <v>676</v>
+        <v>395</v>
       </c>
       <c r="C57">
         <f t="shared" ref="C57" si="14">C55-C56</f>
-        <v>564</v>
+        <v>264</v>
       </c>
       <c r="D57">
         <f t="shared" ref="D57" si="15">D55-D56</f>
-        <v>423</v>
-      </c>
-      <c r="F57" s="7"/>
+        <v>132</v>
+      </c>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58">
-        <f>ROUND(B56*Computation!$B$34,0)</f>
-        <v>635</v>
+        <f>ROUND(B56*Computation!$B$25,0)</f>
+        <v>371</v>
       </c>
       <c r="C58">
-        <f>ROUND(C56*Computation!$B$34,0)</f>
-        <v>529</v>
+        <f>ROUND(C56*Computation!$B$25,0)</f>
+        <v>247</v>
       </c>
       <c r="D58">
-        <f>ROUND(D56*Computation!$B$34,0)</f>
-        <v>397</v>
-      </c>
-      <c r="F58" s="7"/>
+        <f>ROUND(D56*Computation!$B$25,0)</f>
+        <v>124</v>
+      </c>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B59">
         <f>B56-B58</f>
-        <v>423</v>
+        <v>248</v>
       </c>
       <c r="C59">
         <f t="shared" ref="C59" si="16">C56-C58</f>
-        <v>352</v>
+        <v>165</v>
       </c>
       <c r="D59">
         <f t="shared" ref="D59" si="17">D56-D58</f>
-        <v>264</v>
-      </c>
-      <c r="F59" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60">
-        <f>ROUND(B57*Computation!$B$34,0)</f>
-        <v>406</v>
+        <f>ROUND(B57*Computation!$B$25,0)</f>
+        <v>237</v>
       </c>
       <c r="C60">
-        <f>ROUND(C57*Computation!$B$34,0)</f>
-        <v>338</v>
+        <f>ROUND(C57*Computation!$B$25,0)</f>
+        <v>158</v>
       </c>
       <c r="D60">
-        <f>ROUND(D57*Computation!$B$34,0)</f>
-        <v>254</v>
+        <f>ROUND(D57*Computation!$B$25,0)</f>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61">
         <f>B57-B60</f>
-        <v>270</v>
+        <v>158</v>
       </c>
       <c r="C61">
         <f t="shared" ref="C61" si="18">C57-C60</f>
-        <v>226</v>
+        <v>106</v>
       </c>
       <c r="D61">
         <f t="shared" ref="D61" si="19">D57-D60</f>
-        <v>169</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62">
         <f>SUM(B60:B61)</f>
-        <v>676</v>
+        <v>395</v>
       </c>
       <c r="C62">
         <f t="shared" ref="C62" si="20">SUM(C60:C61)</f>
-        <v>564</v>
+        <v>264</v>
       </c>
       <c r="D62">
         <f t="shared" ref="D62" si="21">SUM(D60:D61)</f>
-        <v>423</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64" s="18">
+      <c r="A64" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="26">
+        <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="26">
+        <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D64" s="18">
+      <c r="D64" s="26">
+        <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E64" s="18" t="s">
-        <v>82</v>
+      <c r="E64" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B65">
-        <f>ROUND(Computation!$D$15*Computation!B29,0)+C65</f>
-        <v>1779</v>
+        <f>ROUND(E65*Computation!B20,0)+C65</f>
+        <v>1026</v>
       </c>
       <c r="C65">
-        <f>ROUND(Computation!$D$15*Computation!B30,0)+D65</f>
-        <v>1483</v>
+        <f>ROUND(E65*Computation!B21,0)+D65</f>
+        <v>684</v>
       </c>
       <c r="D65">
-        <f>ROUND(Computation!$D$15*Computation!B31,0)</f>
-        <v>1112</v>
+        <f>ROUND(E65*Computation!B22,0)</f>
+        <v>342</v>
       </c>
       <c r="E65">
-        <f>ROUND(Computation!$D$15,0)</f>
-        <v>2470</v>
+        <f>ROUND(Computation!$E$6,0)</f>
+        <v>3422</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B66">
         <f>ROUND(B65*'Static Data'!$B$4,0)</f>
-        <v>1245</v>
+        <v>718</v>
       </c>
       <c r="C66">
         <f>ROUND(C65*'Static Data'!$B$4,0)</f>
-        <v>1038</v>
+        <v>479</v>
       </c>
       <c r="D66">
         <f>ROUND(D65*'Static Data'!$B$4,0)</f>
-        <v>778</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B67">
         <f>B65-B66</f>
-        <v>534</v>
+        <v>308</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67" si="22">C65-C66</f>
-        <v>445</v>
+        <v>205</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67" si="23">D65-D66</f>
-        <v>334</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68">
-        <f>ROUND(B66*Computation!$B$34,0)</f>
-        <v>747</v>
+        <f>ROUND(B66*Computation!$B$25,0)</f>
+        <v>431</v>
       </c>
       <c r="C68">
-        <f>ROUND(C66*Computation!$B$34,0)</f>
-        <v>623</v>
+        <f>ROUND(C66*Computation!$B$25,0)</f>
+        <v>287</v>
       </c>
       <c r="D68">
-        <f>ROUND(D66*Computation!$B$34,0)</f>
-        <v>467</v>
+        <f>ROUND(D66*Computation!$B$25,0)</f>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B69">
         <f>B66-B68</f>
-        <v>498</v>
+        <v>287</v>
       </c>
       <c r="C69">
         <f t="shared" ref="C69" si="24">C66-C68</f>
-        <v>415</v>
+        <v>192</v>
       </c>
       <c r="D69">
         <f t="shared" ref="D69" si="25">D66-D68</f>
-        <v>311</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B70">
-        <f>ROUND(B67*Computation!$B$34,0)</f>
-        <v>320</v>
+        <f>ROUND(B67*Computation!$B$25,0)</f>
+        <v>185</v>
       </c>
       <c r="C70">
-        <f>ROUND(C67*Computation!$B$34,0)</f>
-        <v>267</v>
+        <f>ROUND(C67*Computation!$B$25,0)</f>
+        <v>123</v>
       </c>
       <c r="D70">
-        <f>ROUND(D67*Computation!$B$34,0)</f>
-        <v>200</v>
+        <f>ROUND(D67*Computation!$B$25,0)</f>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71">
         <f>B67-B70</f>
-        <v>214</v>
+        <v>123</v>
       </c>
       <c r="C71">
         <f t="shared" ref="C71" si="26">C67-C70</f>
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="D71">
         <f t="shared" ref="D71" si="27">D67-D70</f>
-        <v>134</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72">
         <f>SUM(B70:B71)</f>
-        <v>534</v>
+        <v>308</v>
       </c>
       <c r="C72">
         <f t="shared" ref="C72" si="28">SUM(C70:C71)</f>
-        <v>445</v>
+        <v>205</v>
       </c>
       <c r="D72">
         <f t="shared" ref="D72" si="29">SUM(D70:D71)</f>
-        <v>334</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B74" s="18">
+      <c r="A74" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B74" s="26">
+        <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C74" s="18">
+      <c r="C74" s="26">
+        <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D74" s="18">
+      <c r="D74" s="26">
+        <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E74" s="18" t="s">
-        <v>82</v>
+      <c r="E74" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B75">
-        <f>ROUND(Computation!$D$16*Computation!B29,0)+C75</f>
-        <v>1296</v>
+        <f>ROUND(E75*Computation!B20,0)+C75</f>
+        <v>747</v>
       </c>
       <c r="C75">
-        <f>ROUND(Computation!$D$16*Computation!B30,0)+D75</f>
-        <v>1080</v>
+        <f>ROUND(E75*Computation!B21,0)+D75</f>
+        <v>498</v>
       </c>
       <c r="D75">
-        <f>ROUND(Computation!$D$16*Computation!B31,0)</f>
-        <v>810</v>
+        <f>ROUND(E75*Computation!B22,0)</f>
+        <v>249</v>
       </c>
       <c r="E75">
-        <f>ROUND(Computation!$D$16,0)</f>
-        <v>1800</v>
+        <f>ROUND(Computation!$E$7,0)</f>
+        <v>2494</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B76">
         <f>ROUND(B75*'Static Data'!$B$5,0)</f>
-        <v>985</v>
+        <v>568</v>
       </c>
       <c r="C76">
         <f>ROUND(C75*'Static Data'!$B$5,0)</f>
-        <v>821</v>
+        <v>378</v>
       </c>
       <c r="D76">
         <f>ROUND(D75*'Static Data'!$B$5,0)</f>
-        <v>616</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B77">
         <f>B75-B76</f>
-        <v>311</v>
+        <v>179</v>
       </c>
       <c r="C77">
         <f t="shared" ref="C77" si="30">C75-C76</f>
-        <v>259</v>
+        <v>120</v>
       </c>
       <c r="D77">
         <f t="shared" ref="D77" si="31">D75-D76</f>
-        <v>194</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B78">
-        <f>ROUND(B76*Computation!$B$34,0)</f>
-        <v>591</v>
+        <f>ROUND(B76*Computation!$B$25,0)</f>
+        <v>341</v>
       </c>
       <c r="C78">
-        <f>ROUND(C76*Computation!$B$34,0)</f>
-        <v>493</v>
+        <f>ROUND(C76*Computation!$B$25,0)</f>
+        <v>227</v>
       </c>
       <c r="D78">
-        <f>ROUND(D76*Computation!$B$34,0)</f>
-        <v>370</v>
+        <f>ROUND(D76*Computation!$B$25,0)</f>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B79">
         <f>B76-B78</f>
-        <v>394</v>
+        <v>227</v>
       </c>
       <c r="C79">
         <f t="shared" ref="C79" si="32">C76-C78</f>
-        <v>328</v>
+        <v>151</v>
       </c>
       <c r="D79">
         <f t="shared" ref="D79" si="33">D76-D78</f>
-        <v>246</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B80">
-        <f>ROUND(B77*Computation!$B$34,0)</f>
-        <v>187</v>
+        <f>ROUND(B77*Computation!$B$25,0)</f>
+        <v>107</v>
       </c>
       <c r="C80">
-        <f>ROUND(C77*Computation!$B$34,0)</f>
-        <v>155</v>
+        <f>ROUND(C77*Computation!$B$25,0)</f>
+        <v>72</v>
       </c>
       <c r="D80">
-        <f>ROUND(D77*Computation!$B$34,0)</f>
-        <v>116</v>
+        <f>ROUND(D77*Computation!$B$25,0)</f>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B81">
         <f>B77-B80</f>
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C81">
         <f t="shared" ref="C81" si="34">C77-C80</f>
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="D81">
         <f t="shared" ref="D81" si="35">D77-D80</f>
-        <v>78</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B82">
         <f>SUM(B80:B81)</f>
-        <v>311</v>
+        <v>179</v>
       </c>
       <c r="C82">
         <f t="shared" ref="C82" si="36">SUM(C80:C81)</f>
-        <v>259</v>
+        <v>120</v>
       </c>
       <c r="D82">
         <f t="shared" ref="D82" si="37">SUM(D80:D81)</f>
-        <v>194</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B84" s="18">
+      <c r="A84" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="26">
+        <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C84" s="18">
+      <c r="C84" s="26">
+        <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D84" s="18">
+      <c r="D84" s="26">
+        <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E84" s="18" t="s">
-        <v>82</v>
+      <c r="E84" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85">
-        <f>ROUND(Computation!$D$17*Computation!B29,0)+C85</f>
-        <v>1424</v>
+        <f>ROUND(E85*Computation!B20,0)+C85</f>
+        <v>849</v>
       </c>
       <c r="C85">
-        <f>ROUND(Computation!$D$17*Computation!B30,0)+D85</f>
-        <v>1187</v>
+        <f>ROUND(E85*Computation!B21,0)+D85</f>
+        <v>566</v>
       </c>
       <c r="D85">
-        <f>ROUND(Computation!$D$17*Computation!B31,0)</f>
-        <v>890</v>
+        <f>ROUND(E85*Computation!B22,0)</f>
+        <v>283</v>
       </c>
       <c r="E85">
-        <f>ROUND(Computation!$D$17,0)</f>
-        <v>1978</v>
+        <f>ROUND(Computation!$E$8,0)</f>
+        <v>2830</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86">
         <f>ROUND(B85*'Static Data'!$B$6,0)</f>
-        <v>1125</v>
+        <v>671</v>
       </c>
       <c r="C86">
         <f>ROUND(C85*'Static Data'!$B$6,0)</f>
-        <v>938</v>
+        <v>447</v>
       </c>
       <c r="D86">
         <f>ROUND(D85*'Static Data'!$B$6,0)</f>
-        <v>703</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87">
         <f>B85-B86</f>
-        <v>299</v>
+        <v>178</v>
       </c>
       <c r="C87">
         <f t="shared" ref="C87" si="38">C85-C86</f>
-        <v>249</v>
+        <v>119</v>
       </c>
       <c r="D87">
         <f t="shared" ref="D87" si="39">D85-D86</f>
-        <v>187</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88">
-        <f>ROUND(B86*Computation!$B$34,0)</f>
-        <v>675</v>
+        <f>ROUND(B86*Computation!$B$25,0)</f>
+        <v>403</v>
       </c>
       <c r="C88">
-        <f>ROUND(C86*Computation!$B$34,0)</f>
-        <v>563</v>
+        <f>ROUND(C86*Computation!$B$25,0)</f>
+        <v>268</v>
       </c>
       <c r="D88">
-        <f>ROUND(D86*Computation!$B$34,0)</f>
-        <v>422</v>
+        <f>ROUND(D86*Computation!$B$25,0)</f>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89">
         <f>B86-B88</f>
-        <v>450</v>
+        <v>268</v>
       </c>
       <c r="C89">
         <f t="shared" ref="C89" si="40">C86-C88</f>
-        <v>375</v>
+        <v>179</v>
       </c>
       <c r="D89">
         <f t="shared" ref="D89" si="41">D86-D88</f>
-        <v>281</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90">
-        <f>ROUND(B87*Computation!$B$34,0)</f>
-        <v>179</v>
+        <f>ROUND(B87*Computation!$B$25,0)</f>
+        <v>107</v>
       </c>
       <c r="C90">
-        <f>ROUND(C87*Computation!$B$34,0)</f>
-        <v>149</v>
+        <f>ROUND(C87*Computation!$B$25,0)</f>
+        <v>71</v>
       </c>
       <c r="D90">
-        <f>ROUND(D87*Computation!$B$34,0)</f>
-        <v>112</v>
+        <f>ROUND(D87*Computation!$B$25,0)</f>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <f>B87-B90</f>
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="C91">
         <f t="shared" ref="C91" si="42">C87-C90</f>
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="D91">
         <f t="shared" ref="D91" si="43">D87-D90</f>
-        <v>75</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92">
         <f>SUM(B90:B91)</f>
-        <v>299</v>
+        <v>178</v>
       </c>
       <c r="C92">
         <f t="shared" ref="C92" si="44">SUM(C90:C91)</f>
-        <v>249</v>
+        <v>119</v>
       </c>
       <c r="D92">
         <f t="shared" ref="D92" si="45">SUM(D90:D91)</f>
-        <v>187</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+    <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="D94" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="E94" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -4216,18 +3978,18 @@
       </c>
       <c r="B95">
         <f>B42</f>
-        <v>592</v>
-      </c>
-      <c r="C95" s="23">
+        <v>342</v>
+      </c>
+      <c r="C95" s="21">
         <v>1542</v>
       </c>
       <c r="D95" s="1">
-        <f>Computation!E21</f>
-        <v>1.5360983102918587E-3</v>
+        <f>Computation!E12</f>
+        <v>1.1061946902654867E-3</v>
       </c>
       <c r="E95">
         <f>ROUND(B95*(1+D95),0)</f>
-        <v>593</v>
+        <v>342</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -4236,18 +3998,18 @@
       </c>
       <c r="B96">
         <f>B52</f>
-        <v>1297</v>
-      </c>
-      <c r="C96" s="23">
+        <v>760</v>
+      </c>
+      <c r="C96" s="21">
         <v>920</v>
       </c>
       <c r="D96" s="1">
-        <f>Computation!E22</f>
-        <v>3.7936772046589018E-2</v>
+        <f>Computation!E13</f>
+        <v>3.7862449077402348E-2</v>
       </c>
       <c r="E96">
         <f t="shared" ref="E96:E100" si="46">ROUND(B96*(1+D96),0)</f>
-        <v>1346</v>
+        <v>789</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -4256,18 +4018,18 @@
       </c>
       <c r="B97">
         <f>B62</f>
-        <v>676</v>
-      </c>
-      <c r="C97" s="23">
+        <v>395</v>
+      </c>
+      <c r="C97" s="21">
         <v>909</v>
       </c>
       <c r="D97" s="1">
-        <f>Computation!E23</f>
-        <v>3.795966785290629E-2</v>
+        <f>Computation!E14</f>
+        <v>3.7870159453302958E-2</v>
       </c>
       <c r="E97">
         <f t="shared" si="46"/>
-        <v>702</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -4276,18 +4038,18 @@
       </c>
       <c r="B98">
         <f>B72</f>
-        <v>534</v>
-      </c>
-      <c r="C98" s="23">
+        <v>308</v>
+      </c>
+      <c r="C98" s="21">
         <v>876</v>
       </c>
       <c r="D98" s="1">
-        <f>Computation!E24</f>
-        <v>-2.0712510356255178E-2</v>
+        <f>Computation!E15</f>
+        <v>-2.0578586340590517E-2</v>
       </c>
       <c r="E98">
         <f t="shared" si="46"/>
-        <v>523</v>
+        <v>302</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -4296,18 +4058,18 @@
       </c>
       <c r="B99">
         <f>B82</f>
-        <v>311</v>
-      </c>
-      <c r="C99" s="23">
+        <v>179</v>
+      </c>
+      <c r="C99" s="21">
         <v>641</v>
       </c>
       <c r="D99" s="1">
-        <f>Computation!E25</f>
-        <v>-2.1034678794769755E-2</v>
+        <f>Computation!E16</f>
+        <v>-2.0875972165370446E-2</v>
       </c>
       <c r="E99">
         <f t="shared" si="46"/>
-        <v>304</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -4316,43 +4078,43 @@
       </c>
       <c r="B100">
         <f>B92</f>
-        <v>299</v>
-      </c>
-      <c r="C100" s="23">
+        <v>178</v>
+      </c>
+      <c r="C100" s="21">
         <v>618</v>
       </c>
       <c r="D100" s="1">
-        <f>Computation!E26</f>
-        <v>0.12494632889652212</v>
+        <f>Computation!E17</f>
+        <v>0.12519319938176199</v>
       </c>
       <c r="E100">
         <f t="shared" si="46"/>
-        <v>336</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>101</v>
-      </c>
-      <c r="B102" s="22">
+        <v>100</v>
+      </c>
+      <c r="B102" s="20">
         <v>2024</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="23">
+        <v>101</v>
+      </c>
+      <c r="B103" s="21">
         <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1">
         <f>AVERAGE(D95:D100)</f>
-        <v>2.6771946325880727E-2</v>
+        <v>2.6762907349461972E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up Tam exporter for webapp integration along w/ the template
</commit_message>
<xml_diff>
--- a/xls/templates/tam-template.xlsx
+++ b/xls/templates/tam-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E42E1E-4C66-5A4A-8FBF-12F0E42DFF24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B67BE7-DFB2-8E4A-A60F-FD60E106EEFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33260" windowHeight="20440" activeTab="2" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
+    <workbookView xWindow="27000" yWindow="740" windowWidth="37000" windowHeight="15540" activeTab="3" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Zip Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>Rent Stats</t>
   </si>
@@ -216,18 +216,9 @@
     <t>City, State</t>
   </si>
   <si>
-    <t>Phoenix, AZ</t>
-  </si>
-  <si>
     <t>Coordinates</t>
   </si>
   <si>
-    <t>Radius</t>
-  </si>
-  <si>
-    <t>Radius Units</t>
-  </si>
-  <si>
     <t>mi</t>
   </si>
   <si>
@@ -385,6 +376,33 @@
   </si>
   <si>
     <t>Pop Total</t>
+  </si>
+  <si>
+    <t>End of RTI</t>
+  </si>
+  <si>
+    <t>TAM Type</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>Target RTI</t>
+  </si>
+  <si>
+    <t>Max RTI</t>
+  </si>
+  <si>
+    <t>Lower Step</t>
+  </si>
+  <si>
+    <t>Upper Step</t>
+  </si>
+  <si>
+    <t>Step Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +526,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -518,7 +548,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -526,8 +556,10 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -564,8 +596,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="8"/>
+    <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="11" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35"/>
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Good" xfId="4" builtinId="26"/>
@@ -1435,36 +1475,36 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>105</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>106</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>107</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>109</v>
-      </c>
-      <c r="G9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1650,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059DB5A-4215-0640-95EF-B3BB098332D1}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2102,13 +2142,13 @@
         <v>53</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2193,7 +2233,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B29" s="23">
         <v>10000</v>
@@ -2206,10 +2246,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36708BF2-1F90-C543-A265-0490C92231C9}">
-  <dimension ref="A1:Q104"/>
+  <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2230,109 +2270,115 @@
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="21">
-        <v>33.484937100000003</v>
+        <v>0</v>
       </c>
       <c r="C3" s="21">
-        <v>-112.0856505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
+      <c r="B5" s="2">
+        <f>Computation!B29</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2">
-        <f>Computation!B29</f>
-        <v>10000</v>
+        <f>SUM(B103:B108)</f>
+        <v>2162</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="2">
-        <f>SUM(B95:B100)</f>
-        <v>2162</v>
+        <v>64</v>
+      </c>
+      <c r="B7" s="19">
+        <f>SUM(C103:C108)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="19">
-        <f>SUM(C95:C100)</f>
-        <v>5506</v>
+        <v>65</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(E103:E108)</f>
+        <v>2218</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="2">
-        <f>SUM(E95:E100)</f>
-        <v>2218</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="A11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="22">
+        <v>0</v>
+      </c>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>1</v>
+      <c r="A12" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="B12" s="22">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="22">
-        <v>750</v>
-      </c>
-      <c r="C13" s="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="22">
-        <v>900</v>
-      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -2340,8 +2386,11 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>70</v>
+      <c r="A16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0.33329999999999999</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2349,15 +2398,16 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>73</v>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="30">
+        <f>MAX(0.55, B16+0.2)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E17" t="s">
+        <v>122</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2365,15 +2415,13 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="20">
-        <v>0</v>
-      </c>
-      <c r="C18" s="20">
-        <v>0.12</v>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="30">
+        <f>B16/2.5</f>
+        <v>0.13331999999999999</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2381,15 +2429,13 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="20">
-        <v>0.12</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0.24</v>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="30">
+        <f>(B17-B16)/2.5</f>
+        <v>8.6680000000000021E-2</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2397,15 +2443,18 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="20">
-        <v>0.24</v>
-      </c>
-      <c r="C20" s="20">
-        <v>0.35</v>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2413,15 +2462,20 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="20">
-        <v>0.35</v>
-      </c>
-      <c r="C21" s="20">
-        <v>0.45</v>
+        <v>71</v>
+      </c>
+      <c r="B21" s="32">
+        <v>0</v>
+      </c>
+      <c r="C21" s="32">
+        <f>ROUND(B21+B18,2)</f>
+        <v>0.13</v>
+      </c>
+      <c r="D21" s="33">
+        <f>B18</f>
+        <v>0.13331999999999999</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2429,15 +2483,21 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="20">
-        <v>0.45</v>
-      </c>
-      <c r="C22" s="20">
-        <v>0.55000000000000004</v>
+        <v>72</v>
+      </c>
+      <c r="B22" s="32">
+        <f>C21+0.01</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C22" s="32">
+        <f>ROUND(B22+B18,2)</f>
+        <v>0.27</v>
+      </c>
+      <c r="D22" s="33">
+        <f>B18</f>
+        <v>0.13331999999999999</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -2445,42 +2505,21 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23">
-        <v>15000</v>
-      </c>
-      <c r="C23">
-        <v>20000</v>
-      </c>
-      <c r="D23">
-        <v>25000</v>
-      </c>
-      <c r="E23">
-        <v>30000</v>
-      </c>
-      <c r="F23">
-        <v>35000</v>
-      </c>
-      <c r="G23">
-        <v>40000</v>
-      </c>
-      <c r="H23">
-        <v>45000</v>
-      </c>
-      <c r="I23">
-        <v>50000</v>
-      </c>
-      <c r="J23">
-        <v>55000</v>
-      </c>
-      <c r="K23">
-        <v>60000</v>
-      </c>
-      <c r="L23">
-        <v>65000</v>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="31">
+        <f>C22+0.01</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C23" s="31">
+        <f>B23+(B18/2)+(B19/2)</f>
+        <v>0.39</v>
+      </c>
+      <c r="D23" s="33">
+        <f>(B18+B19)/2</f>
+        <v>0.11000000000000001</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -2488,53 +2527,21 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>500</v>
-      </c>
-      <c r="B24" s="4">
-        <f>$A24/(B$23/12)</f>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="31">
+        <f>C23+0.01</f>
         <v>0.4</v>
       </c>
-      <c r="C24" s="4">
-        <f t="shared" ref="C24:L24" si="0">$A24/(C$23/12)</f>
-        <v>0.3</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="E24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.17142857142857143</v>
-      </c>
-      <c r="G24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="J24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.1090909090909091</v>
-      </c>
-      <c r="K24" s="4">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="L24" s="4">
-        <f t="shared" si="0"/>
-        <v>9.2307692307692299E-2</v>
+      <c r="C24" s="31">
+        <f>ROUND(B24+B19,2)</f>
+        <v>0.49</v>
+      </c>
+      <c r="D24" s="33">
+        <f>B19</f>
+        <v>8.6680000000000021E-2</v>
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -2542,53 +2549,21 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>600</v>
-      </c>
-      <c r="B25" s="4">
-        <f t="shared" ref="B25:L32" si="1">$A25/(B$23/12)</f>
-        <v>0.48</v>
-      </c>
-      <c r="C25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="D25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="E25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.20571428571428574</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="J25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.13090909090909092</v>
-      </c>
-      <c r="K25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="L25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.11076923076923076</v>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="31">
+        <f>C24+0.01</f>
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="31">
+        <f>ROUND(B25+B19, 2)</f>
+        <v>0.59</v>
+      </c>
+      <c r="D25" s="33">
+        <f>B19</f>
+        <v>8.6680000000000021E-2</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -2596,1524 +2571,2106 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>700</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.42</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.33599999999999997</v>
-      </c>
-      <c r="E26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24000000000000002</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.21</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.18666666666666668</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16799999999999998</v>
-      </c>
-      <c r="J26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.15272727272727274</v>
-      </c>
-      <c r="K26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12923076923076923</v>
-      </c>
-      <c r="M26" s="3"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>15000</v>
+      </c>
+      <c r="C26">
+        <v>20000</v>
+      </c>
+      <c r="D26">
+        <v>20000</v>
+      </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>500</v>
+      </c>
+      <c r="B27" s="28">
+        <f>IF(B$26&lt;&gt;"", IF($A27&lt;&gt;"",$A27/(B$26/12),""), "")</f>
+        <v>0.4</v>
+      </c>
+      <c r="C27" s="28">
+        <f t="shared" ref="C27:Q27" si="0">IF(C$26&lt;&gt;"", IF($A27&lt;&gt;"",$A27/(C$26/12),""), "")</f>
+        <v>0.3</v>
+      </c>
+      <c r="D27" s="28">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="E27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>600</v>
+      </c>
+      <c r="B28" s="28">
+        <f t="shared" ref="B28:Q40" si="1">IF(B$26&lt;&gt;"", IF($A28&lt;&gt;"",$A28/(B$26/12),""), "")</f>
+        <v>0.48</v>
+      </c>
+      <c r="C28" s="28">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+      <c r="D28" s="28">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+      <c r="E28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q28" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>700</v>
+      </c>
+      <c r="B29" s="28">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C29" s="28">
+        <f t="shared" si="1"/>
+        <v>0.42</v>
+      </c>
+      <c r="D29" s="28">
+        <f t="shared" si="1"/>
+        <v>0.42</v>
+      </c>
+      <c r="E29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q29" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>800</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B30" s="28">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C30" s="28">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="D27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.38399999999999995</v>
-      </c>
-      <c r="E27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2742857142857143</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.21333333333333335</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.19199999999999998</v>
-      </c>
-      <c r="J27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.17454545454545456</v>
-      </c>
-      <c r="K27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
-      </c>
-      <c r="L27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.14769230769230768</v>
-      </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>900</v>
-      </c>
-      <c r="B28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
-      </c>
-      <c r="C28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.53999999999999992</v>
-      </c>
-      <c r="D28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.432</v>
-      </c>
-      <c r="E28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="F28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.30857142857142861</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26999999999999996</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.216</v>
-      </c>
-      <c r="J28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.19636363636363638</v>
-      </c>
-      <c r="K28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="L28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16615384615384615</v>
-      </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1000</v>
-      </c>
-      <c r="B29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="C29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-      <c r="D29" s="4">
+      <c r="D30" s="28">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="E29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="F29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.34285714285714286</v>
-      </c>
-      <c r="G29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="I29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="J29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2181818181818182</v>
-      </c>
-      <c r="K29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="L29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1846153846153846</v>
-      </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>1100</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.88</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.65999999999999992</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.52799999999999991</v>
-      </c>
-      <c r="E30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.37714285714285717</v>
-      </c>
-      <c r="G30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.32999999999999996</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.29333333333333333</v>
-      </c>
-      <c r="I30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26399999999999996</v>
-      </c>
-      <c r="J30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24000000000000002</v>
-      </c>
-      <c r="K30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22</v>
-      </c>
-      <c r="L30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.20307692307692307</v>
-      </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>1200</v>
-      </c>
-      <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.96</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
-      </c>
-      <c r="D31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="E31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-      <c r="F31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.41142857142857148</v>
-      </c>
-      <c r="G31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-      <c r="I31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="J31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26181818181818184</v>
-      </c>
-      <c r="K31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="L31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22153846153846152</v>
-      </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>1300</v>
-      </c>
-      <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>1.04</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.77999999999999992</v>
-      </c>
-      <c r="D32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.624</v>
-      </c>
-      <c r="E32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.52</v>
-      </c>
-      <c r="F32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.44571428571428573</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.38999999999999996</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.34666666666666668</v>
-      </c>
-      <c r="I32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.312</v>
-      </c>
-      <c r="J32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.28363636363636363</v>
-      </c>
-      <c r="K32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
-      </c>
-      <c r="L32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-    </row>
-    <row r="34" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="26">
+      <c r="E30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q30" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q31" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q32" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q33" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q34" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q35" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q38" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q40" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="R40" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+    </row>
+    <row r="42" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C42" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D42" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35">
-        <f>ROUND(E35*Computation!B20,0)+C35</f>
+      <c r="E42" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43">
+        <f>ROUND(E43*Computation!B20,0)+C43</f>
         <v>543</v>
       </c>
-      <c r="C35">
-        <f>ROUND(E35*Computation!B21,0)+D35</f>
+      <c r="C43">
+        <f>ROUND(E43*Computation!B21,0)+D43</f>
         <v>362</v>
       </c>
-      <c r="D35">
-        <f>ROUND(E35*Computation!B22,0)</f>
+      <c r="D43">
+        <f>ROUND(E43*Computation!B22,0)</f>
         <v>181</v>
       </c>
-      <c r="E35">
+      <c r="E43">
         <f>ROUND(Computation!$E$3,0)</f>
         <v>1806</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36">
-        <f>ROUND(B35*'Static Data'!$B$2,0)</f>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44">
+        <f>ROUND(B43*'Static Data'!$B$2,0)</f>
         <v>201</v>
       </c>
-      <c r="C36">
-        <f>ROUND(C35*'Static Data'!$B$2,0)</f>
+      <c r="C44">
+        <f>ROUND(C43*'Static Data'!$B$2,0)</f>
         <v>134</v>
       </c>
-      <c r="D36">
-        <f>ROUND(D35*'Static Data'!$B$2,0)</f>
+      <c r="D44">
+        <f>ROUND(D43*'Static Data'!$B$2,0)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37">
-        <f>B35-B36</f>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45">
+        <f>B43-B44</f>
         <v>342</v>
       </c>
-      <c r="C37">
-        <f t="shared" ref="C37:D37" si="2">C35-C36</f>
+      <c r="C45">
+        <f t="shared" ref="C45:D45" si="2">C43-C44</f>
         <v>228</v>
       </c>
-      <c r="D37">
+      <c r="D45">
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38">
-        <f>ROUND(B36*Computation!$B$25,0)</f>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46">
+        <f>ROUND(B44*Computation!$B$25,0)</f>
         <v>121</v>
       </c>
-      <c r="C38">
-        <f>ROUND(C36*Computation!$B$25,0)</f>
+      <c r="C46">
+        <f>ROUND(C44*Computation!$B$25,0)</f>
         <v>80</v>
       </c>
-      <c r="D38">
-        <f>ROUND(D36*Computation!$B$25,0)</f>
+      <c r="D46">
+        <f>ROUND(D44*Computation!$B$25,0)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39">
-        <f>B36-B38</f>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47">
+        <f>B44-B46</f>
         <v>80</v>
       </c>
-      <c r="C39">
-        <f t="shared" ref="C39:D39" si="3">C36-C38</f>
+      <c r="C47">
+        <f t="shared" ref="C47:D47" si="3">C44-C46</f>
         <v>54</v>
       </c>
-      <c r="D39">
+      <c r="D47">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40">
-        <f>ROUND(B37*Computation!$B$25,0)</f>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48">
+        <f>ROUND(B45*Computation!$B$25,0)</f>
         <v>205</v>
       </c>
-      <c r="C40">
-        <f>ROUND(C37*Computation!$B$25,0)</f>
+      <c r="C48">
+        <f>ROUND(C45*Computation!$B$25,0)</f>
         <v>137</v>
       </c>
-      <c r="D40">
-        <f>ROUND(D37*Computation!$B$25,0)</f>
+      <c r="D48">
+        <f>ROUND(D45*Computation!$B$25,0)</f>
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41">
-        <f>B37-B40</f>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49">
+        <f>B45-B48</f>
         <v>137</v>
       </c>
-      <c r="C41">
-        <f t="shared" ref="C41:D41" si="4">C37-C40</f>
+      <c r="C49">
+        <f t="shared" ref="C49:D49" si="4">C45-C48</f>
         <v>91</v>
       </c>
-      <c r="D41">
+      <c r="D49">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42">
-        <f>SUM(B40:B41)</f>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50">
+        <f>SUM(B48:B49)</f>
         <v>342</v>
       </c>
-      <c r="C42">
-        <f t="shared" ref="C42:D42" si="5">SUM(C40:C41)</f>
+      <c r="C50">
+        <f t="shared" ref="C50:D50" si="5">SUM(C48:C49)</f>
         <v>228</v>
       </c>
-      <c r="D42">
+      <c r="D50">
         <f t="shared" si="5"/>
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="26">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C44" s="26">
+      <c r="C52" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D52" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E44" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45">
-        <f>ROUND(E45*Computation!B20,0)+C45</f>
+      <c r="E52" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53">
+        <f>ROUND(E53*Computation!B20,0)+C53</f>
         <v>1206</v>
       </c>
-      <c r="C45">
-        <f>ROUND(E45*Computation!B21,0)+D45</f>
+      <c r="C53">
+        <f>ROUND(E53*Computation!B21,0)+D53</f>
         <v>804</v>
       </c>
-      <c r="D45">
-        <f>ROUND(E45*Computation!B22,0)</f>
+      <c r="D53">
+        <f>ROUND(E53*Computation!B22,0)</f>
         <v>402</v>
       </c>
-      <c r="E45">
+      <c r="E53">
         <f>ROUND(Computation!$E$4,0)</f>
         <v>4015</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54">
+        <f>ROUND(B53*'Static Data'!$B$2,0)</f>
+        <v>446</v>
+      </c>
+      <c r="C54">
+        <f>ROUND(C53*'Static Data'!$B$2,0)</f>
+        <v>297</v>
+      </c>
+      <c r="D54">
+        <f>ROUND(D53*'Static Data'!$B$2,0)</f>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <f>B53-B54</f>
+        <v>760</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55" si="6">C53-C54</f>
+        <v>507</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ref="D55" si="7">D53-D54</f>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56">
+        <f>ROUND(B54*Computation!$B$25,0)</f>
+        <v>268</v>
+      </c>
+      <c r="C56">
+        <f>ROUND(C54*Computation!$B$25,0)</f>
+        <v>178</v>
+      </c>
+      <c r="D56">
+        <f>ROUND(D54*Computation!$B$25,0)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>83</v>
       </c>
-      <c r="B46">
-        <f>ROUND(B45*'Static Data'!$B$2,0)</f>
-        <v>446</v>
-      </c>
-      <c r="C46">
-        <f>ROUND(C45*'Static Data'!$B$2,0)</f>
-        <v>297</v>
-      </c>
-      <c r="D46">
-        <f>ROUND(D45*'Static Data'!$B$2,0)</f>
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B57">
+        <f>B54-B56</f>
+        <v>178</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57" si="8">C54-C56</f>
+        <v>119</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57" si="9">D54-D56</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>84</v>
       </c>
-      <c r="B47">
-        <f>B45-B46</f>
+      <c r="B58">
+        <f>ROUND(B55*Computation!$B$25,0)</f>
+        <v>456</v>
+      </c>
+      <c r="C58">
+        <f>ROUND(C55*Computation!$B$25,0)</f>
+        <v>304</v>
+      </c>
+      <c r="D58">
+        <f>ROUND(D55*Computation!$B$25,0)</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59">
+        <f>B55-B58</f>
+        <v>304</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ref="C59" si="10">C55-C58</f>
+        <v>203</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ref="D59" si="11">D55-D58</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60">
+        <f>SUM(B58:B59)</f>
         <v>760</v>
       </c>
-      <c r="C47">
-        <f t="shared" ref="C47" si="6">C45-C46</f>
+      <c r="C60">
+        <f t="shared" ref="C60" si="12">SUM(C58:C59)</f>
         <v>507</v>
       </c>
-      <c r="D47">
-        <f t="shared" ref="D47" si="7">D45-D46</f>
+      <c r="D60">
+        <f t="shared" ref="D60" si="13">SUM(D58:D59)</f>
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48">
-        <f>ROUND(B46*Computation!$B$25,0)</f>
-        <v>268</v>
-      </c>
-      <c r="C48">
-        <f>ROUND(C46*Computation!$B$25,0)</f>
-        <v>178</v>
-      </c>
-      <c r="D48">
-        <f>ROUND(D46*Computation!$B$25,0)</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49">
-        <f>B46-B48</f>
-        <v>178</v>
-      </c>
-      <c r="C49">
-        <f t="shared" ref="C49" si="8">C46-C48</f>
-        <v>119</v>
-      </c>
-      <c r="D49">
-        <f t="shared" ref="D49" si="9">D46-D48</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50">
-        <f>ROUND(B47*Computation!$B$25,0)</f>
-        <v>456</v>
-      </c>
-      <c r="C50">
-        <f>ROUND(C47*Computation!$B$25,0)</f>
-        <v>304</v>
-      </c>
-      <c r="D50">
-        <f>ROUND(D47*Computation!$B$25,0)</f>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B51">
-        <f>B47-B50</f>
-        <v>304</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51" si="10">C47-C50</f>
-        <v>203</v>
-      </c>
-      <c r="D51">
-        <f t="shared" ref="D51" si="11">D47-D50</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52">
-        <f>SUM(B50:B51)</f>
-        <v>760</v>
-      </c>
-      <c r="C52">
-        <f t="shared" ref="C52" si="12">SUM(C50:C51)</f>
-        <v>507</v>
-      </c>
-      <c r="D52">
-        <f t="shared" ref="D52" si="13">SUM(D50:D51)</f>
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="26">
+      <c r="B62" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C62" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D54" s="26">
+      <c r="D62" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55">
-        <f>ROUND(E55*Computation!B20,0)+C55</f>
+      <c r="E62" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63">
+        <f>ROUND(E63*Computation!B20,0)+C63</f>
         <v>1014</v>
       </c>
-      <c r="C55">
-        <f>ROUND(E55*Computation!B21,0)+D55</f>
+      <c r="C63">
+        <f>ROUND(E63*Computation!B21,0)+D63</f>
         <v>676</v>
       </c>
-      <c r="D55">
-        <f>ROUND(E55*Computation!B22,0)</f>
+      <c r="D63">
+        <f>ROUND(E63*Computation!B22,0)</f>
         <v>338</v>
       </c>
-      <c r="E55">
+      <c r="E63">
         <f>ROUND(Computation!$E$5,0)</f>
         <v>3379</v>
       </c>
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64">
+        <f>ROUND(B63*'Static Data'!$B$3,0)</f>
+        <v>619</v>
+      </c>
+      <c r="C64">
+        <f>ROUND(C63*'Static Data'!$B$3,0)</f>
+        <v>412</v>
+      </c>
+      <c r="D64">
+        <f>ROUND(D63*'Static Data'!$B$3,0)</f>
+        <v>206</v>
+      </c>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65">
+        <f>B63-B64</f>
+        <v>395</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ref="C65" si="14">C63-C64</f>
+        <v>264</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ref="D65" si="15">D63-D64</f>
+        <v>132</v>
+      </c>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66">
+        <f>ROUND(B64*Computation!$B$25,0)</f>
+        <v>371</v>
+      </c>
+      <c r="C66">
+        <f>ROUND(C64*Computation!$B$25,0)</f>
+        <v>247</v>
+      </c>
+      <c r="D66">
+        <f>ROUND(D64*Computation!$B$25,0)</f>
+        <v>124</v>
+      </c>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>83</v>
       </c>
-      <c r="B56">
-        <f>ROUND(B55*'Static Data'!$B$3,0)</f>
-        <v>619</v>
-      </c>
-      <c r="C56">
-        <f>ROUND(C55*'Static Data'!$B$3,0)</f>
-        <v>412</v>
-      </c>
-      <c r="D56">
-        <f>ROUND(D55*'Static Data'!$B$3,0)</f>
-        <v>206</v>
-      </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B67">
+        <f>B64-B66</f>
+        <v>248</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67" si="16">C64-C66</f>
+        <v>165</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67" si="17">D64-D66</f>
+        <v>82</v>
+      </c>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>84</v>
       </c>
-      <c r="B57">
-        <f>B55-B56</f>
+      <c r="B68">
+        <f>ROUND(B65*Computation!$B$25,0)</f>
+        <v>237</v>
+      </c>
+      <c r="C68">
+        <f>ROUND(C65*Computation!$B$25,0)</f>
+        <v>158</v>
+      </c>
+      <c r="D68">
+        <f>ROUND(D65*Computation!$B$25,0)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69">
+        <f>B65-B68</f>
+        <v>158</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ref="C69" si="18">C65-C68</f>
+        <v>106</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69" si="19">D65-D68</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70">
+        <f>SUM(B68:B69)</f>
         <v>395</v>
       </c>
-      <c r="C57">
-        <f t="shared" ref="C57" si="14">C55-C56</f>
+      <c r="C70">
+        <f t="shared" ref="C70" si="20">SUM(C68:C69)</f>
         <v>264</v>
       </c>
-      <c r="D57">
-        <f t="shared" ref="D57" si="15">D55-D56</f>
+      <c r="D70">
+        <f t="shared" ref="D70" si="21">SUM(D68:D69)</f>
         <v>132</v>
       </c>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>85</v>
-      </c>
-      <c r="B58">
-        <f>ROUND(B56*Computation!$B$25,0)</f>
-        <v>371</v>
-      </c>
-      <c r="C58">
-        <f>ROUND(C56*Computation!$B$25,0)</f>
-        <v>247</v>
-      </c>
-      <c r="D58">
-        <f>ROUND(D56*Computation!$B$25,0)</f>
-        <v>124</v>
-      </c>
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B59">
-        <f>B56-B58</f>
-        <v>248</v>
-      </c>
-      <c r="C59">
-        <f t="shared" ref="C59" si="16">C56-C58</f>
-        <v>165</v>
-      </c>
-      <c r="D59">
-        <f t="shared" ref="D59" si="17">D56-D58</f>
-        <v>82</v>
-      </c>
-      <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60">
-        <f>ROUND(B57*Computation!$B$25,0)</f>
-        <v>237</v>
-      </c>
-      <c r="C60">
-        <f>ROUND(C57*Computation!$B$25,0)</f>
-        <v>158</v>
-      </c>
-      <c r="D60">
-        <f>ROUND(D57*Computation!$B$25,0)</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61">
-        <f>B57-B60</f>
-        <v>158</v>
-      </c>
-      <c r="C61">
-        <f t="shared" ref="C61" si="18">C57-C60</f>
-        <v>106</v>
-      </c>
-      <c r="D61">
-        <f t="shared" ref="D61" si="19">D57-D60</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B62">
-        <f>SUM(B60:B61)</f>
-        <v>395</v>
-      </c>
-      <c r="C62">
-        <f t="shared" ref="C62" si="20">SUM(C60:C61)</f>
-        <v>264</v>
-      </c>
-      <c r="D62">
-        <f t="shared" ref="D62" si="21">SUM(D60:D61)</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="26">
+      <c r="B72" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C64" s="26">
+      <c r="C72" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D64" s="26">
+      <c r="D72" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E64" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65">
-        <f>ROUND(E65*Computation!B20,0)+C65</f>
+      <c r="E72" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73">
+        <f>ROUND(E73*Computation!B20,0)+C73</f>
         <v>1026</v>
       </c>
-      <c r="C65">
-        <f>ROUND(E65*Computation!B21,0)+D65</f>
+      <c r="C73">
+        <f>ROUND(E73*Computation!B21,0)+D73</f>
         <v>684</v>
       </c>
-      <c r="D65">
-        <f>ROUND(E65*Computation!B22,0)</f>
+      <c r="D73">
+        <f>ROUND(E73*Computation!B22,0)</f>
         <v>342</v>
       </c>
-      <c r="E65">
+      <c r="E73">
         <f>ROUND(Computation!$E$6,0)</f>
         <v>3422</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74">
+        <f>ROUND(B73*'Static Data'!$B$4,0)</f>
+        <v>718</v>
+      </c>
+      <c r="C74">
+        <f>ROUND(C73*'Static Data'!$B$4,0)</f>
+        <v>479</v>
+      </c>
+      <c r="D74">
+        <f>ROUND(D73*'Static Data'!$B$4,0)</f>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75">
+        <f>B73-B74</f>
+        <v>308</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75" si="22">C73-C74</f>
+        <v>205</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75" si="23">D73-D74</f>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76">
+        <f>ROUND(B74*Computation!$B$25,0)</f>
+        <v>431</v>
+      </c>
+      <c r="C76">
+        <f>ROUND(C74*Computation!$B$25,0)</f>
+        <v>287</v>
+      </c>
+      <c r="D76">
+        <f>ROUND(D74*Computation!$B$25,0)</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>83</v>
       </c>
-      <c r="B66">
-        <f>ROUND(B65*'Static Data'!$B$4,0)</f>
-        <v>718</v>
-      </c>
-      <c r="C66">
-        <f>ROUND(C65*'Static Data'!$B$4,0)</f>
-        <v>479</v>
-      </c>
-      <c r="D66">
-        <f>ROUND(D65*'Static Data'!$B$4,0)</f>
-        <v>239</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B77">
+        <f>B74-B76</f>
+        <v>287</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ref="C77" si="24">C74-C76</f>
+        <v>192</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77" si="25">D74-D76</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>84</v>
       </c>
-      <c r="B67">
-        <f>B65-B66</f>
+      <c r="B78">
+        <f>ROUND(B75*Computation!$B$25,0)</f>
+        <v>185</v>
+      </c>
+      <c r="C78">
+        <f>ROUND(C75*Computation!$B$25,0)</f>
+        <v>123</v>
+      </c>
+      <c r="D78">
+        <f>ROUND(D75*Computation!$B$25,0)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79">
+        <f>B75-B78</f>
+        <v>123</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ref="C79" si="26">C75-C78</f>
+        <v>82</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ref="D79" si="27">D75-D78</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80">
+        <f>SUM(B78:B79)</f>
         <v>308</v>
       </c>
-      <c r="C67">
-        <f t="shared" ref="C67" si="22">C65-C66</f>
+      <c r="C80">
+        <f t="shared" ref="C80" si="28">SUM(C78:C79)</f>
         <v>205</v>
       </c>
-      <c r="D67">
-        <f t="shared" ref="D67" si="23">D65-D66</f>
+      <c r="D80">
+        <f t="shared" ref="D80" si="29">SUM(D78:D79)</f>
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68">
-        <f>ROUND(B66*Computation!$B$25,0)</f>
-        <v>431</v>
-      </c>
-      <c r="C68">
-        <f>ROUND(C66*Computation!$B$25,0)</f>
-        <v>287</v>
-      </c>
-      <c r="D68">
-        <f>ROUND(D66*Computation!$B$25,0)</f>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>86</v>
-      </c>
-      <c r="B69">
-        <f>B66-B68</f>
-        <v>287</v>
-      </c>
-      <c r="C69">
-        <f t="shared" ref="C69" si="24">C66-C68</f>
-        <v>192</v>
-      </c>
-      <c r="D69">
-        <f t="shared" ref="D69" si="25">D66-D68</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70">
-        <f>ROUND(B67*Computation!$B$25,0)</f>
-        <v>185</v>
-      </c>
-      <c r="C70">
-        <f>ROUND(C67*Computation!$B$25,0)</f>
-        <v>123</v>
-      </c>
-      <c r="D70">
-        <f>ROUND(D67*Computation!$B$25,0)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71">
-        <f>B67-B70</f>
-        <v>123</v>
-      </c>
-      <c r="C71">
-        <f t="shared" ref="C71" si="26">C67-C70</f>
-        <v>82</v>
-      </c>
-      <c r="D71">
-        <f t="shared" ref="D71" si="27">D67-D70</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>89</v>
-      </c>
-      <c r="B72">
-        <f>SUM(B70:B71)</f>
-        <v>308</v>
-      </c>
-      <c r="C72">
-        <f t="shared" ref="C72" si="28">SUM(C70:C71)</f>
-        <v>205</v>
-      </c>
-      <c r="D72">
-        <f t="shared" ref="D72" si="29">SUM(D70:D71)</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" s="26">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C74" s="26">
+      <c r="C82" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D74" s="26">
+      <c r="D82" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E74" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75">
-        <f>ROUND(E75*Computation!B20,0)+C75</f>
+      <c r="E82" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <f>ROUND(E83*Computation!B20,0)+C83</f>
         <v>747</v>
       </c>
-      <c r="C75">
-        <f>ROUND(E75*Computation!B21,0)+D75</f>
+      <c r="C83">
+        <f>ROUND(E83*Computation!B21,0)+D83</f>
         <v>498</v>
       </c>
-      <c r="D75">
-        <f>ROUND(E75*Computation!B22,0)</f>
+      <c r="D83">
+        <f>ROUND(E83*Computation!B22,0)</f>
         <v>249</v>
       </c>
-      <c r="E75">
+      <c r="E83">
         <f>ROUND(Computation!$E$7,0)</f>
         <v>2494</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <f>ROUND(B83*'Static Data'!$B$5,0)</f>
+        <v>568</v>
+      </c>
+      <c r="C84">
+        <f>ROUND(C83*'Static Data'!$B$5,0)</f>
+        <v>378</v>
+      </c>
+      <c r="D84">
+        <f>ROUND(D83*'Static Data'!$B$5,0)</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85">
+        <f>B83-B84</f>
+        <v>179</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ref="C85" si="30">C83-C84</f>
+        <v>120</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ref="D85" si="31">D83-D84</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86">
+        <f>ROUND(B84*Computation!$B$25,0)</f>
+        <v>341</v>
+      </c>
+      <c r="C86">
+        <f>ROUND(C84*Computation!$B$25,0)</f>
+        <v>227</v>
+      </c>
+      <c r="D86">
+        <f>ROUND(D84*Computation!$B$25,0)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>83</v>
       </c>
-      <c r="B76">
-        <f>ROUND(B75*'Static Data'!$B$5,0)</f>
-        <v>568</v>
-      </c>
-      <c r="C76">
-        <f>ROUND(C75*'Static Data'!$B$5,0)</f>
-        <v>378</v>
-      </c>
-      <c r="D76">
-        <f>ROUND(D75*'Static Data'!$B$5,0)</f>
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B87">
+        <f>B84-B86</f>
+        <v>227</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ref="C87" si="32">C84-C86</f>
+        <v>151</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ref="D87" si="33">D84-D86</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>84</v>
       </c>
-      <c r="B77">
-        <f>B75-B76</f>
+      <c r="B88">
+        <f>ROUND(B85*Computation!$B$25,0)</f>
+        <v>107</v>
+      </c>
+      <c r="C88">
+        <f>ROUND(C85*Computation!$B$25,0)</f>
+        <v>72</v>
+      </c>
+      <c r="D88">
+        <f>ROUND(D85*Computation!$B$25,0)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <f>B85-B88</f>
+        <v>72</v>
+      </c>
+      <c r="C89">
+        <f t="shared" ref="C89" si="34">C85-C88</f>
+        <v>48</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ref="D89" si="35">D85-D88</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+      <c r="B90">
+        <f>SUM(B88:B89)</f>
         <v>179</v>
       </c>
-      <c r="C77">
-        <f t="shared" ref="C77" si="30">C75-C76</f>
+      <c r="C90">
+        <f t="shared" ref="C90" si="36">SUM(C88:C89)</f>
         <v>120</v>
       </c>
-      <c r="D77">
-        <f t="shared" ref="D77" si="31">D75-D76</f>
+      <c r="D90">
+        <f t="shared" ref="D90" si="37">SUM(D88:D89)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78">
-        <f>ROUND(B76*Computation!$B$25,0)</f>
-        <v>341</v>
-      </c>
-      <c r="C78">
-        <f>ROUND(C76*Computation!$B$25,0)</f>
-        <v>227</v>
-      </c>
-      <c r="D78">
-        <f>ROUND(D76*Computation!$B$25,0)</f>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79">
-        <f>B76-B78</f>
-        <v>227</v>
-      </c>
-      <c r="C79">
-        <f t="shared" ref="C79" si="32">C76-C78</f>
-        <v>151</v>
-      </c>
-      <c r="D79">
-        <f t="shared" ref="D79" si="33">D76-D78</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80">
-        <f>ROUND(B77*Computation!$B$25,0)</f>
-        <v>107</v>
-      </c>
-      <c r="C80">
-        <f>ROUND(C77*Computation!$B$25,0)</f>
-        <v>72</v>
-      </c>
-      <c r="D80">
-        <f>ROUND(D77*Computation!$B$25,0)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81">
-        <f>B77-B80</f>
-        <v>72</v>
-      </c>
-      <c r="C81">
-        <f t="shared" ref="C81" si="34">C77-C80</f>
-        <v>48</v>
-      </c>
-      <c r="D81">
-        <f t="shared" ref="D81" si="35">D77-D80</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>89</v>
-      </c>
-      <c r="B82">
-        <f>SUM(B80:B81)</f>
-        <v>179</v>
-      </c>
-      <c r="C82">
-        <f t="shared" ref="C82" si="36">SUM(C80:C81)</f>
-        <v>120</v>
-      </c>
-      <c r="D82">
-        <f t="shared" ref="D82" si="37">SUM(D80:D81)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="26">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="26">
         <f>Computation!$A$20</f>
         <v>25000</v>
       </c>
-      <c r="C84" s="26">
+      <c r="C92" s="26">
         <f>Computation!$A$21</f>
         <v>35000</v>
       </c>
-      <c r="D84" s="26">
+      <c r="D92" s="26">
         <f>Computation!$A$22</f>
         <v>45000</v>
       </c>
-      <c r="E84" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85">
-        <f>ROUND(E85*Computation!B20,0)+C85</f>
+      <c r="E92" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93">
+        <f>ROUND(E93*Computation!B20,0)+C93</f>
         <v>849</v>
       </c>
-      <c r="C85">
-        <f>ROUND(E85*Computation!B21,0)+D85</f>
+      <c r="C93">
+        <f>ROUND(E93*Computation!B21,0)+D93</f>
         <v>566</v>
       </c>
-      <c r="D85">
-        <f>ROUND(E85*Computation!B22,0)</f>
+      <c r="D93">
+        <f>ROUND(E93*Computation!B22,0)</f>
         <v>283</v>
       </c>
-      <c r="E85">
+      <c r="E93">
         <f>ROUND(Computation!$E$8,0)</f>
         <v>2830</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86">
-        <f>ROUND(B85*'Static Data'!$B$6,0)</f>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>80</v>
+      </c>
+      <c r="B94">
+        <f>ROUND(B93*'Static Data'!$B$6,0)</f>
         <v>671</v>
       </c>
-      <c r="C86">
-        <f>ROUND(C85*'Static Data'!$B$6,0)</f>
+      <c r="C94">
+        <f>ROUND(C93*'Static Data'!$B$6,0)</f>
         <v>447</v>
       </c>
-      <c r="D86">
-        <f>ROUND(D85*'Static Data'!$B$6,0)</f>
+      <c r="D94">
+        <f>ROUND(D93*'Static Data'!$B$6,0)</f>
         <v>224</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87">
-        <f>B85-B86</f>
-        <v>178</v>
-      </c>
-      <c r="C87">
-        <f t="shared" ref="C87" si="38">C85-C86</f>
-        <v>119</v>
-      </c>
-      <c r="D87">
-        <f t="shared" ref="D87" si="39">D85-D86</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88">
-        <f>ROUND(B86*Computation!$B$25,0)</f>
-        <v>403</v>
-      </c>
-      <c r="C88">
-        <f>ROUND(C86*Computation!$B$25,0)</f>
-        <v>268</v>
-      </c>
-      <c r="D88">
-        <f>ROUND(D86*Computation!$B$25,0)</f>
-        <v>134</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89">
-        <f>B86-B88</f>
-        <v>268</v>
-      </c>
-      <c r="C89">
-        <f t="shared" ref="C89" si="40">C86-C88</f>
-        <v>179</v>
-      </c>
-      <c r="D89">
-        <f t="shared" ref="D89" si="41">D86-D88</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90">
-        <f>ROUND(B87*Computation!$B$25,0)</f>
-        <v>107</v>
-      </c>
-      <c r="C90">
-        <f>ROUND(C87*Computation!$B$25,0)</f>
-        <v>71</v>
-      </c>
-      <c r="D90">
-        <f>ROUND(D87*Computation!$B$25,0)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>88</v>
-      </c>
-      <c r="B91">
-        <f>B87-B90</f>
-        <v>71</v>
-      </c>
-      <c r="C91">
-        <f t="shared" ref="C91" si="42">C87-C90</f>
-        <v>48</v>
-      </c>
-      <c r="D91">
-        <f t="shared" ref="D91" si="43">D87-D90</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92">
-        <f>SUM(B90:B91)</f>
-        <v>178</v>
-      </c>
-      <c r="C92">
-        <f t="shared" ref="C92" si="44">SUM(C90:C91)</f>
-        <v>119</v>
-      </c>
-      <c r="D92">
-        <f t="shared" ref="D92" si="45">SUM(D90:D91)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95">
+        <f>B93-B94</f>
+        <v>178</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95" si="38">C93-C94</f>
+        <v>119</v>
+      </c>
+      <c r="D95">
+        <f t="shared" ref="D95" si="39">D93-D94</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>82</v>
+      </c>
+      <c r="B96">
+        <f>ROUND(B94*Computation!$B$25,0)</f>
+        <v>403</v>
+      </c>
+      <c r="C96">
+        <f>ROUND(C94*Computation!$B$25,0)</f>
+        <v>268</v>
+      </c>
+      <c r="D96">
+        <f>ROUND(D94*Computation!$B$25,0)</f>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97">
+        <f>B94-B96</f>
+        <v>268</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ref="C97" si="40">C94-C96</f>
+        <v>179</v>
+      </c>
+      <c r="D97">
+        <f t="shared" ref="D97" si="41">D94-D96</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>84</v>
+      </c>
+      <c r="B98">
+        <f>ROUND(B95*Computation!$B$25,0)</f>
+        <v>107</v>
+      </c>
+      <c r="C98">
+        <f>ROUND(C95*Computation!$B$25,0)</f>
+        <v>71</v>
+      </c>
+      <c r="D98">
+        <f>ROUND(D95*Computation!$B$25,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99">
+        <f>B95-B98</f>
+        <v>71</v>
+      </c>
+      <c r="C99">
+        <f t="shared" ref="C99" si="42">C95-C98</f>
+        <v>48</v>
+      </c>
+      <c r="D99">
+        <f t="shared" ref="D99" si="43">D95-D98</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100">
+        <f>SUM(B98:B99)</f>
+        <v>178</v>
+      </c>
+      <c r="C100">
+        <f t="shared" ref="C100" si="44">SUM(C98:C99)</f>
+        <v>119</v>
+      </c>
+      <c r="D100">
+        <f t="shared" ref="D100" si="45">SUM(D98:D99)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>6</v>
       </c>
-      <c r="B95">
-        <f>B42</f>
+      <c r="B103">
+        <f>B50</f>
         <v>342</v>
       </c>
-      <c r="C95" s="21">
-        <v>1542</v>
-      </c>
-      <c r="D95" s="1">
+      <c r="C103" s="21">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1">
         <f>Computation!E12</f>
         <v>1.1061946902654867E-3</v>
       </c>
-      <c r="E95">
-        <f>ROUND(B95*(1+D95),0)</f>
+      <c r="E103">
+        <f>ROUND(B103*(1+D103),0)</f>
         <v>342</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>7</v>
       </c>
-      <c r="B96">
-        <f>B52</f>
+      <c r="B104">
+        <f>B60</f>
         <v>760</v>
       </c>
-      <c r="C96" s="21">
-        <v>920</v>
-      </c>
-      <c r="D96" s="1">
+      <c r="C104" s="21">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1">
         <f>Computation!E13</f>
         <v>3.7862449077402348E-2</v>
       </c>
-      <c r="E96">
-        <f t="shared" ref="E96:E100" si="46">ROUND(B96*(1+D96),0)</f>
+      <c r="E104">
+        <f t="shared" ref="E104:E108" si="46">ROUND(B104*(1+D104),0)</f>
         <v>789</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>8</v>
       </c>
-      <c r="B97">
-        <f>B62</f>
+      <c r="B105">
+        <f>B70</f>
         <v>395</v>
       </c>
-      <c r="C97" s="21">
-        <v>909</v>
-      </c>
-      <c r="D97" s="1">
+      <c r="C105" s="21">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1">
         <f>Computation!E14</f>
         <v>3.7870159453302958E-2</v>
       </c>
-      <c r="E97">
+      <c r="E105">
         <f t="shared" si="46"/>
         <v>410</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="B98">
-        <f>B72</f>
+      <c r="B106">
+        <f>B80</f>
         <v>308</v>
       </c>
-      <c r="C98" s="21">
-        <v>876</v>
-      </c>
-      <c r="D98" s="1">
+      <c r="C106" s="21">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1">
         <f>Computation!E15</f>
         <v>-2.0578586340590517E-2</v>
       </c>
-      <c r="E98">
+      <c r="E106">
         <f t="shared" si="46"/>
         <v>302</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>10</v>
       </c>
-      <c r="B99">
-        <f>B82</f>
+      <c r="B107">
+        <f>B90</f>
         <v>179</v>
       </c>
-      <c r="C99" s="21">
-        <v>641</v>
-      </c>
-      <c r="D99" s="1">
+      <c r="C107" s="21">
+        <v>0</v>
+      </c>
+      <c r="D107" s="1">
         <f>Computation!E16</f>
         <v>-2.0875972165370446E-2</v>
       </c>
-      <c r="E99">
+      <c r="E107">
         <f t="shared" si="46"/>
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>11</v>
       </c>
-      <c r="B100">
-        <f>B92</f>
+      <c r="B108">
+        <f>B100</f>
         <v>178</v>
       </c>
-      <c r="C100" s="21">
-        <v>618</v>
-      </c>
-      <c r="D100" s="1">
+      <c r="C108" s="21">
+        <v>0</v>
+      </c>
+      <c r="D108" s="1">
         <f>Computation!E17</f>
         <v>0.12519319938176199</v>
       </c>
-      <c r="E100">
+      <c r="E108">
         <f t="shared" si="46"/>
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="20">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>97</v>
+      </c>
+      <c r="B110" s="20">
         <v>2024</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>101</v>
-      </c>
-      <c r="B103" s="21">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="1">
-        <f>AVERAGE(D95:D100)</f>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>98</v>
+      </c>
+      <c r="B111" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>99</v>
+      </c>
+      <c r="B112" s="1">
+        <f>AVERAGE(D103:D108)</f>
         <v>2.6762907349461972E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding a version tab to the TAM
</commit_message>
<xml_diff>
--- a/xls/templates/tam-template.xlsx
+++ b/xls/templates/tam-template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B67BE7-DFB2-8E4A-A60F-FD60E106EEFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7EFF30-55F1-CA4E-A4A0-12CEC86509B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27000" yWindow="740" windowWidth="37000" windowHeight="15540" activeTab="3" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
+    <workbookView xWindow="27000" yWindow="740" windowWidth="37000" windowHeight="15540" activeTab="4" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Zip Data" sheetId="1" r:id="rId1"/>
     <sheet name="Static Data" sheetId="4" r:id="rId2"/>
     <sheet name="Computation" sheetId="2" r:id="rId3"/>
     <sheet name="Output" sheetId="3" r:id="rId4"/>
+    <sheet name="VERSION" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="124">
   <si>
     <t>Rent Stats</t>
   </si>
@@ -403,18 +404,22 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -559,7 +564,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -593,15 +598,16 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="8"/>
     <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="11" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
@@ -942,10 +948,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -975,11 +981,11 @@
       <c r="C4" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1280,10 +1286,10 @@
       <c r="D32" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
@@ -2248,7 +2254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36708BF2-1F90-C543-A265-0490C92231C9}">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -2389,7 +2395,7 @@
       <c r="A16" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <v>0.33329999999999999</v>
       </c>
       <c r="M16" s="3"/>
@@ -2402,7 +2408,7 @@
       <c r="A17" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <f>MAX(0.55, B16+0.2)</f>
         <v>0.55000000000000004</v>
       </c>
@@ -2419,7 +2425,7 @@
       <c r="A18" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <f>B16/2.5</f>
         <v>0.13331999999999999</v>
       </c>
@@ -2433,7 +2439,7 @@
       <c r="A19" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <f>(B17-B16)/2.5</f>
         <v>8.6680000000000021E-2</v>
       </c>
@@ -2466,14 +2472,14 @@
       <c r="A21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>0</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <f>ROUND(B21+B18,2)</f>
         <v>0.13</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <f>B18</f>
         <v>0.13331999999999999</v>
       </c>
@@ -2487,15 +2493,15 @@
       <c r="A22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="31">
         <f>C21+0.01</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <f>ROUND(B22+B18,2)</f>
         <v>0.27</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <f>B18</f>
         <v>0.13331999999999999</v>
       </c>
@@ -2509,15 +2515,15 @@
       <c r="A23" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="30">
         <f>C22+0.01</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="30">
         <f>B23+(B18/2)+(B19/2)</f>
         <v>0.39</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="32">
         <f>(B18+B19)/2</f>
         <v>0.11000000000000001</v>
       </c>
@@ -2531,15 +2537,15 @@
       <c r="A24" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="30">
         <f>C23+0.01</f>
         <v>0.4</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="30">
         <f>ROUND(B24+B19,2)</f>
         <v>0.49</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <f>B19</f>
         <v>8.6680000000000021E-2</v>
       </c>
@@ -2553,15 +2559,15 @@
       <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="30">
         <f>C24+0.01</f>
         <v>0.5</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="30">
         <f>ROUND(B25+B19, 2)</f>
         <v>0.59</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="32">
         <f>B19</f>
         <v>8.6680000000000021E-2</v>
       </c>
@@ -2593,71 +2599,71 @@
       <c r="A27">
         <v>500</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="27">
         <f>IF(B$26&lt;&gt;"", IF($A27&lt;&gt;"",$A27/(B$26/12),""), "")</f>
         <v>0.4</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="27">
         <f t="shared" ref="C27:Q27" si="0">IF(C$26&lt;&gt;"", IF($A27&lt;&gt;"",$A27/(C$26/12),""), "")</f>
         <v>0.3</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="27">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="E27" s="28" t="str">
+      <c r="E27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="28" t="str">
+      <c r="F27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G27" s="28" t="str">
+      <c r="G27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H27" s="28" t="str">
+      <c r="H27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I27" s="28" t="str">
+      <c r="I27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J27" s="28" t="str">
+      <c r="J27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K27" s="28" t="str">
+      <c r="K27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L27" s="28" t="str">
+      <c r="L27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M27" s="28" t="str">
+      <c r="M27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N27" s="28" t="str">
+      <c r="N27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O27" s="28" t="str">
+      <c r="O27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P27" s="28" t="str">
+      <c r="P27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q27" s="28" t="str">
+      <c r="Q27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R27" s="29" t="s">
+      <c r="R27" s="28" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2665,67 +2671,67 @@
       <c r="A28">
         <v>600</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="27">
         <f t="shared" ref="B28:Q40" si="1">IF(B$26&lt;&gt;"", IF($A28&lt;&gt;"",$A28/(B$26/12),""), "")</f>
         <v>0.48</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="27">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="27">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P28" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q28" s="28" t="str">
+      <c r="E28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q28" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2734,67 +2740,67 @@
       <c r="A29">
         <v>700</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="27">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="27">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="27">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="E29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P29" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q29" s="28" t="str">
+      <c r="E29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P29" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q29" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2803,731 +2809,731 @@
       <c r="A30">
         <v>800</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="27">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="27">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="27">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="E30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P30" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q30" s="28" t="str">
+      <c r="E30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P30" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q30" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P31" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q31" s="28" t="str">
+      <c r="B31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P31" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q31" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P32" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q32" s="28" t="str">
+      <c r="B32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P32" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q32" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P33" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q33" s="28" t="str">
+      <c r="B33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P33" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q33" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P34" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q34" s="28" t="str">
+      <c r="B34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P34" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q34" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q35" s="28" t="str">
+      <c r="B35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P35" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q35" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P36" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q36" s="28" t="str">
+      <c r="B36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P36" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q36" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P37" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q37" s="28" t="str">
+      <c r="B37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P37" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q37" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P38" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q38" s="28" t="str">
+      <c r="B38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P38" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q38" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P39" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q39" s="28" t="str">
+      <c r="B39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P39" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q39" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="P40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="R40" s="29" t="s">
+      <c r="B40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q40" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="R40" s="28" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4677,4 +4683,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED48FEA-52D6-9F43-B50B-F7F61862367C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="34">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement data, make sure it is income-major
</commit_message>
<xml_diff>
--- a/xls/templates/tam-template.xlsx
+++ b/xls/templates/tam-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/dev/psl/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645EB961-380F-BF4E-9AC7-2ED60F86D8A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C7DC22-0BAE-8C44-957E-8BB87B8A406C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
+    <workbookView xWindow="1680" yWindow="820" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{314BF30B-A255-874B-AE37-BE104BEBF62F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Zip Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
   <si>
     <t>Rent Stats</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>spreadsheet_version</t>
+  </si>
+  <si>
+    <t>Example, WA</t>
   </si>
 </sst>
 </file>
@@ -2258,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36708BF2-1F90-C543-A265-0490C92231C9}">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,7 +2283,9 @@
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="21" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4693,7 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED48FEA-52D6-9F43-B50B-F7F61862367C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>